<commit_message>
bugfix in percentPPI trester
</commit_message>
<xml_diff>
--- a/Peakfinder Results/RESULTS_MTT.xlsx
+++ b/Peakfinder Results/RESULTS_MTT.xlsx
@@ -744,52 +744,52 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[12, 12, 12, 12, 12]</t>
+          <t>[12, 12, 12, 12]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[18, 18, 18, 18, 18]</t>
+          <t>[18, 18, 18, 18]</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[44, 67, 66, 65, 75]</t>
+          <t>[67, 66, 65, 75]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[44.6, 67.74, 66.39999999999999, 65.06, 75.12]</t>
+          <t>[67.74, 66.39999999999999, 65.06, 75.12]</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>[36.55, 65.05999999999999, 63.05, 62.38, 61.03]</t>
+          <t>[65.05999999999999, 63.05, 62.38, 61.03]</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>[16.98, 26.19, 25.75, 24.65, 33.28]</t>
+          <t>[26.19, 25.75, 24.65, 33.28]</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[172.44, 163.9, 178.86, 163.16, 188.34]</t>
+          <t>[163.9, 178.86, 163.16, 188.34]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>[4528.96, 6615.92, 6747.36, 6486.78, 9057.91]</t>
+          <t>[6615.92, 6747.36, 6486.78, 9057.91]</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>[-8.37, -8.37, -8.37, -8.37, -8.37]</t>
+          <t>[-8.37, -8.37, -8.37, -8.37]</t>
         </is>
       </c>
     </row>
@@ -1032,52 +1032,52 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[12, 12, 10, 12, 12]</t>
+          <t>[12, 10, 12, 12]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>[18, 18, 20, 18, 18]</t>
+          <t>[18, 20, 18, 18]</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[60, 64, 63, 71, 56]</t>
+          <t>[64, 63, 71, 56]</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>[60.36, 64.39, 63.38, 70.75999999999999, 56.34]</t>
+          <t>[64.39, 63.38, 70.75999999999999, 56.34]</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>[54.99, 59.36, 63.04, 60.37, 46.28]</t>
+          <t>[59.36, 63.04, 60.37, 46.28]</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>[24.11, 26.16, 23.24, 28.61, 21.29]</t>
+          <t>[26.16, 23.24, 28.61, 21.29]</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>[172.05, 185.31, 143.32, 152.9, 122.82]</t>
+          <t>[185.31, 143.32, 152.9, 122.82]</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>[6352.67, 6897.44, 5685.68, 7378.71, 5299.8]</t>
+          <t>[6897.44, 5685.68, 7378.71, 5299.8]</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>[-10.16, -10.16, -10.16, -10.16, -10.16]</t>
+          <t>[-10.16, -10.16, -10.16, -10.16]</t>
         </is>
       </c>
     </row>
@@ -1248,52 +1248,52 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[12, 12, 12, 14]</t>
+          <t>[12, 12, 14]</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 32]</t>
+          <t>[30, 30, 32]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[18, 18, 18, 18]</t>
+          <t>[18, 18, 18]</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>[34, 57, 51, 14]</t>
+          <t>[57, 51, 14]</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>[34.54, 57.68, 50.98, 13.75]</t>
+          <t>[57.68, 50.98, 13.75]</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>[29.169999999999998, 48.96, 47.629999999999995, 12.08]</t>
+          <t>[48.96, 47.629999999999995, 12.08]</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>[12.89, 21.2, 19.15, 5.15]</t>
+          <t>[21.2, 19.15, 5.15]</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>[129.24, 170.11, 161.29, 89.15]</t>
+          <t>[170.11, 161.29, 89.15]</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>[3312.05, 5511.71, 4935.47, 1300.54]</t>
+          <t>[5511.71, 4935.47, 1300.54]</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>[19.21, 19.21, 19.21, 19.21]</t>
+          <t>[19.21, 19.21, 19.21]</t>
         </is>
       </c>
     </row>
@@ -1608,52 +1608,52 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[12, 12, 12, 14, 12]</t>
+          <t>[12, 12, 14, 12]</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 32, 30]</t>
+          <t>[30, 30, 32, 30]</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>[18, 18, 18, 18, 18]</t>
+          <t>[18, 18, 18, 18]</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>[61, 45, 40, 27, 42]</t>
+          <t>[45, 40, 27, 42]</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>[60.699999999999996, 45.94, 40.91, 27.83, 42.26]</t>
+          <t>[45.94, 40.91, 27.83, 42.26]</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>[48.629999999999995, 45.94, 39.23, 26.15, 39.239999999999995]</t>
+          <t>[45.94, 39.23, 26.15, 39.239999999999995]</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>[24.04, 16.05, 14.9, 9.14, 16.54]</t>
+          <t>[16.05, 14.9, 9.14, 16.54]</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>[154.98, 132.78, 134.34, 128.27, 131.79]</t>
+          <t>[132.78, 134.34, 128.27, 131.79]</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>[6248.64, 3816.49, 3507.26, 2157.15, 3980.36]</t>
+          <t>[3816.49, 3507.26, 2157.15, 3980.36]</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>[23.05, 23.05, 23.05, 23.05, 23.05]</t>
+          <t>[23.05, 23.05, 23.05, 23.05]</t>
         </is>
       </c>
     </row>
@@ -1680,52 +1680,52 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>[12, 12, 12, 12, 12]</t>
+          <t>[12, 12, 12, 12]</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[18, 18, 18, 18, 18]</t>
+          <t>[18, 18, 18, 18]</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>[43, 38, 46, 50, 51]</t>
+          <t>[38, 46, 50, 51]</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>[43.93, 38.57, 45.94, 50.97, 51.98]</t>
+          <t>[38.57, 45.94, 50.97, 51.98]</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>[34.879999999999995, 31.53, 43.26, 46.269999999999996, 50.63999999999999]</t>
+          <t>[31.53, 43.26, 46.269999999999996, 50.63999999999999]</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>[16.98, 15.09, 16.42, 18.9, 20.57]</t>
+          <t>[15.09, 16.42, 18.9, 20.57]</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>[189.65, 144.98, 157.16, 150.82, 166.52]</t>
+          <t>[144.98, 157.16, 150.82, 166.52]</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>[4597.73, 3807.2, 4024.67, 4613.43, 5442.3]</t>
+          <t>[3807.2, 4024.67, 4613.43, 5442.3]</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>[18.8, 18.8, 18.8, 18.8, 18.8]</t>
+          <t>[18.8, 18.8, 18.8, 18.8]</t>
         </is>
       </c>
     </row>
@@ -1824,52 +1824,52 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 10]</t>
+          <t>[10, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[32, 30, 30, 52, 18]</t>
+          <t>[30, 30, 52, 18]</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[22, 20, 20, 42, 8]</t>
+          <t>[20, 20, 42, 8]</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>[123, 142, 167, 224, 157]</t>
+          <t>[142, 167, 224, 157]</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>[123.75, 142.53, 167.34, 177.74, 157.95]</t>
+          <t>[142.53, 167.34, 177.74, 157.95]</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>[118.05, 133.81, 138.17, 191.83, 139.83999999999997]</t>
+          <t>[133.81, 138.17, 191.83, 139.83999999999997]</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>[48.64, 58.69, 73.58, 93.13, 59.9]</t>
+          <t>[58.69, 73.58, 93.13, 59.9]</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>[103.63, 130.47, 150.6, 140.83, 114.34]</t>
+          <t>[130.47, 150.6, 140.83, 114.34]</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>[10724.99, 13970.76, 18301.42, 21306.32, 15288.08]</t>
+          <t>[13970.76, 18301.42, 21306.32, 15288.08]</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>[None, None, None, None, None]</t>
+          <t>[None, None, None, None]</t>
         </is>
       </c>
     </row>
@@ -2256,52 +2256,52 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[10, 10, 10]</t>
+          <t>[10, 10]</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[32, 30, 30]</t>
+          <t>[30, 30]</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>[22, 20, 20]</t>
+          <t>[20, 20]</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>[154, 105, 204]</t>
+          <t>[105, 204]</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>[154.6, 105.3, 203.89]</t>
+          <t>[105.3, 203.89]</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>[154.26, 87.53, 184.10999999999999]</t>
+          <t>[87.53, 184.10999999999999]</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>[59.37, 39.0, 83.7]</t>
+          <t>[39.0, 83.7]</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>[116.2, 96.0, 164.61]</t>
+          <t>[96.0, 164.61]</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>[12739.76, 8681.18, 20472.06]</t>
+          <t>[8681.18, 20472.06]</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>[11.92, 11.92, 11.92]</t>
+          <t>[11.92, 11.92]</t>
         </is>
       </c>
     </row>
@@ -2328,52 +2328,52 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 10]</t>
+          <t>[10, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[86, 30, 30, 30, 52]</t>
+          <t>[30, 30, 30, 52]</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>[76, 20, 20, 20, 42]</t>
+          <t>[20, 20, 20, 42]</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>[120, 127, 165, 136, 133]</t>
+          <t>[127, 165, 136, 133]</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>[119.38, 127.1, 164.99, 136.83, 131.12]</t>
+          <t>[127.1, 164.99, 136.83, 131.12]</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>[117.71, 109.0, 128.78000000000003, 110.34000000000002, 120.73]</t>
+          <t>[109.0, 128.78000000000003, 110.34000000000002, 120.73]</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>[54.16, 47.12, 71.53, 52.71, 60.4]</t>
+          <t>[47.12, 71.53, 52.71, 60.4]</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>[101.42, 96.8, 162.04, 111.61, 147.35]</t>
+          <t>[96.8, 162.04, 111.61, 147.35]</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>[8210.26, 9999.76, 18188.09, 11710.92, 13272.04]</t>
+          <t>[9999.76, 18188.09, 11710.92, 13272.04]</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>[8.65, 8.65, 8.65, 8.65, 8.65]</t>
+          <t>[8.65, 8.65, 8.65, 8.65]</t>
         </is>
       </c>
     </row>
@@ -2544,52 +2544,52 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[12, 12, 10, 10, 10]</t>
+          <t>[12, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>[32, 30, 30, 32, 32]</t>
+          <t>[30, 30, 32, 32]</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>[20, 18, 20, 22, 22]</t>
+          <t>[18, 20, 22, 22]</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>[115, 127, 108, 162, 118]</t>
+          <t>[127, 108, 162, 118]</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>[115.7, 127.77, 108.32, 162.31, 118.72]</t>
+          <t>[127.77, 108.32, 162.31, 118.72]</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>[114.36, 105.64, 94.23, 137.16, 115.03]</t>
+          <t>[105.64, 94.23, 137.16, 115.03]</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>[47.6, 49.32, 43.17, 67.95, 47.58]</t>
+          <t>[49.32, 43.17, 67.95, 47.58]</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>[134.99, 108.66, 103.19, 131.5, 153.62]</t>
+          <t>[108.66, 103.19, 131.5, 153.62]</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>[11293.7, 10939.81, 9719.2, 16274.35, 12165.05]</t>
+          <t>[10939.81, 9719.2, 16274.35, 12165.05]</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>[16.11, 16.11, 16.11, 16.11, 16.11]</t>
+          <t>[16.11, 16.11, 16.11, 16.11]</t>
         </is>
       </c>
     </row>
@@ -3048,52 +3048,52 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[10, 10, 12, 10]</t>
+          <t>[10, 12, 10]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[32, 32, 30, 30]</t>
+          <t>[32, 30, 30]</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>[22, 22, 18, 20]</t>
+          <t>[22, 18, 20]</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>[135, 143, 104, 144]</t>
+          <t>[143, 104, 144]</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>[134.81, 142.86, 104.3, 144.54]</t>
+          <t>[142.86, 104.3, 144.54]</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>[128.78, 120.06, 90.55, 118.38]</t>
+          <t>[120.06, 90.55, 118.38]</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>[49.88, 59.0, 40.63, 58.29]</t>
+          <t>[59.0, 40.63, 58.29]</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>[120.13, 127.95, 120.81, 126.27]</t>
+          <t>[127.95, 120.81, 126.27]</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>[10668.78, 13227.18, 9503.17, 14374.99]</t>
+          <t>[13227.18, 9503.17, 14374.99]</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>[9.91, 9.91, 9.91, 9.91]</t>
+          <t>[9.91, 9.91, 9.91]</t>
         </is>
       </c>
     </row>
@@ -3408,52 +3408,52 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 10]</t>
+          <t>[10, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 20, 20]</t>
+          <t>[20, 20, 20, 20]</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>[124, 141, 133, 145, 96]</t>
+          <t>[124, 133, 145, 96]</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>[124.08, 141.18, 133.47, 145.55, 96.24]</t>
+          <t>[124.08, 133.47, 145.55, 96.24]</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>[122.07000000000001, 137.83, 124.08, 140.85000000000002, 92.89]</t>
+          <t>[122.07000000000001, 124.08, 140.85000000000002, 92.89]</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>[49.84, 52.48, 51.33, 50.35, 39.14]</t>
+          <t>[49.84, 51.33, 50.35, 39.14]</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>[122.13, 96.95, 95.69, 66.81, 142.13]</t>
+          <t>[122.13, 95.69, 66.81, 142.13]</t>
         </is>
       </c>
       <c r="M42" t="inlineStr">
         <is>
-          <t>[11029.49, 10734.89, 10331.9, 9243.37, 10247.06]</t>
+          <t>[11029.49, 10331.9, 9243.37, 10247.06]</t>
         </is>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>[-3.2, -3.2, -3.2, -3.2, -3.2]</t>
+          <t>[-3.2, -3.2, -3.2, -3.2]</t>
         </is>
       </c>
     </row>
@@ -3480,52 +3480,52 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 12, 12]</t>
+          <t>[10, 10, 12, 12]</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[30, 28, 30, 34, 28]</t>
+          <t>[28, 30, 34, 28]</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>[20, 18, 20, 22, 16]</t>
+          <t>[18, 20, 22, 16]</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>[134, 103, 117, 115, 72]</t>
+          <t>[103, 117, 115, 72]</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>[134.47, 102.96, 117.71, 115.02, 72.44]</t>
+          <t>[102.96, 117.71, 115.02, 72.44]</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>[128.44, 83.50999999999999, 117.03999999999999, 113.67999999999999, 59.03]</t>
+          <t>[83.50999999999999, 117.03999999999999, 113.67999999999999, 59.03]</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>[54.83, 38.45, 44.11, 37.15, 27.84]</t>
+          <t>[38.45, 44.11, 37.15, 27.84]</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>[115.31, 86.63, 115.91, 71.56, 145.41]</t>
+          <t>[86.63, 115.91, 71.56, 145.41]</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>[12314.62, 7363.69, 10061.34, 7444.03, 7552.15]</t>
+          <t>[7363.69, 10061.34, 7444.03, 7552.15]</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>[10.85, 10.85, 10.85, 10.85, 10.85]</t>
+          <t>[10.85, 10.85, 10.85, 10.85]</t>
         </is>
       </c>
     </row>
@@ -3624,52 +3624,52 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 10]</t>
+          <t>[10, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 20, 20]</t>
+          <t>[20, 20, 20, 20]</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>[141, 124, 119, 124, 114]</t>
+          <t>[124, 119, 124, 114]</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>[140.85, 124.75, 119.05, 124.08, 114.36]</t>
+          <t>[124.75, 119.05, 124.08, 114.36]</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>[127.44, 119.05, 100.94, 110.33, 114.36]</t>
+          <t>[119.05, 100.94, 110.33, 114.36]</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>[57.22, 46.02, 45.54, 43.38, 45.13]</t>
+          <t>[46.02, 45.54, 43.38, 45.13]</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>[122.36, 102.44, 108.43, 84.41, 137.82]</t>
+          <t>[102.44, 108.43, 84.41, 137.82]</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>[12890.79, 9932.63, 9876.64, 9191.14, 11302.31]</t>
+          <t>[9932.63, 9876.64, 9191.14, 11302.31]</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>[1.84, 1.84, 1.84, 1.84, 1.84]</t>
+          <t>[1.84, 1.84, 1.84, 1.84]</t>
         </is>
       </c>
     </row>
@@ -3984,52 +3984,52 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10]</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[52, 30, 30, 30]</t>
+          <t>[30, 30]</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>[42, 20, 20, 20]</t>
+          <t>[20, 20]</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>[122, 129, 94, 127]</t>
+          <t>[94, 127]</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>[121.4, 129.78, 93.89999999999999, 127.44]</t>
+          <t>[93.89999999999999, 127.44]</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>[108.99, 124.41, 88.53999999999999, 119.73]</t>
+          <t>[88.53999999999999, 119.73]</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>[46.83, 52.96, 35.76, 49.29]</t>
+          <t>[35.76, 49.29]</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>[89.33, 104.92, 106.29, 110.86]</t>
+          <t>[106.29, 110.86]</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>[8488.03, 11191.39, 7800.27, 12050.3]</t>
+          <t>[7800.27, 12050.3]</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>[12.53, 12.53, 12.53, 12.53]</t>
+          <t>[12.53, 12.53]</t>
         </is>
       </c>
     </row>
@@ -4848,52 +4848,52 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 12]</t>
+          <t>[10, 12]</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30]</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 18]</t>
+          <t>[20, 18]</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>[90, 73, 79, 69]</t>
+          <t>[79, 69]</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>[90.21, 73.44, 78.8, 69.08]</t>
+          <t>[78.8, 69.08]</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>[75.44999999999999, 67.39999999999999, 77.46, 68.74]</t>
+          <t>[77.46, 68.74]</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>[40.84, 27.0, 32.61, 25.38]</t>
+          <t>[32.61, 25.38]</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>[200.53, 156.31, 179.24, 140.01]</t>
+          <t>[179.24, 140.01]</t>
         </is>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>[11411.79, 6837.99, 8865.54, 6318.28]</t>
+          <t>[8865.54, 6318.28]</t>
         </is>
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>[1.33, 1.33, 1.33, 1.33]</t>
+          <t>[1.33, 1.33]</t>
         </is>
       </c>
     </row>
@@ -4992,52 +4992,52 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[10, 10, 12, 10, 12]</t>
+          <t>[10, 12, 10, 12]</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>[20, 20, 18, 20, 18]</t>
+          <t>[20, 18, 20, 18]</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>[65, 76, 72, 89, 74]</t>
+          <t>[65, 72, 89, 74]</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>[65.73, 76.13, 72.77, 89.88, 74.11]</t>
+          <t>[65.73, 72.77, 89.88, 74.11]</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>[58.35, 71.1, 66.72999999999999, 77.14, 66.4]</t>
+          <t>[58.35, 66.72999999999999, 77.14, 66.4]</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>[23.7, 29.31, 28.45, 34.54, 28.91]</t>
+          <t>[23.7, 28.45, 34.54, 28.91]</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>[122.89, 161.23, 137.81, 143.4, 147.21]</t>
+          <t>[122.89, 137.81, 143.4, 147.21]</t>
         </is>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>[5801.06, 7427.35, 7201.79, 8789.32, 7239.2]</t>
+          <t>[5801.06, 7201.79, 8789.32, 7239.2]</t>
         </is>
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>[14.99, 14.99, 14.99, 14.99, 14.99]</t>
+          <t>[14.99, 14.99, 14.99, 14.99]</t>
         </is>
       </c>
     </row>
@@ -5352,52 +5352,52 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>[12, 12, 12, 12, 10]</t>
+          <t>[12, 12, 12, 10]</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>[30, 32, 30, 30, 30]</t>
+          <t>[32, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>[18, 20, 18, 18, 20]</t>
+          <t>[20, 18, 18, 20]</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>[78, 59, 70, 77, 65]</t>
+          <t>[59, 70, 77, 65]</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>[77.8, 59.349999999999994, 70.09, 76.78999999999999, 65.05]</t>
+          <t>[59.349999999999994, 70.09, 76.78999999999999, 65.05]</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>[63.72, 53.32, 69.42, 73.44, 61.03]</t>
+          <t>[53.32, 69.42, 73.44, 61.03]</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>[30.27, 24.06, 24.5, 27.32, 25.65]</t>
+          <t>[24.06, 24.5, 27.32, 25.65]</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>[142.81, 146.69, 132.13, 145.25, 144.32]</t>
+          <t>[146.69, 132.13, 145.25, 144.32]</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>[7829.55, 6014.52, 6080.26, 7025.43, 6501.74]</t>
+          <t>[6014.52, 6080.26, 7025.43, 6501.74]</t>
         </is>
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>[15.16, 15.16, 15.16, 15.16, 15.16]</t>
+          <t>[15.16, 15.16, 15.16, 15.16]</t>
         </is>
       </c>
     </row>
@@ -6072,52 +6072,52 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[12, 10, 10, 12]</t>
+          <t>[10, 10, 12]</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>[30, 32, 30, 30]</t>
+          <t>[32, 30, 30]</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>[18, 22, 20, 18]</t>
+          <t>[22, 20, 18]</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>[52, 88, 65, 67]</t>
+          <t>[88, 65, 67]</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>[52.65, 88.53, 65.05, 67.07]</t>
+          <t>[88.53, 65.05, 67.07]</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>[44.94, 73.44, 58.69, 57.68]</t>
+          <t>[73.44, 58.69, 57.68]</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>[20.27, 39.54, 27.45, 28.25]</t>
+          <t>[39.54, 27.45, 28.25]</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>[175.12, 185.42, 155.85, 161.05]</t>
+          <t>[185.42, 155.85, 161.05]</t>
         </is>
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>[5268.38, 10831.95, 7640.38, 7786.04]</t>
+          <t>[10831.95, 7640.38, 7786.04]</t>
         </is>
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>[-1.61, -1.61, -1.61, -1.61]</t>
+          <t>[-1.61, -1.61, -1.61]</t>
         </is>
       </c>
     </row>
@@ -6288,52 +6288,52 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>[10, 12, 10, 10]</t>
+          <t>[12, 10, 10]</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>[32, 32, 30, 30]</t>
+          <t>[32, 30, 30]</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>[22, 20, 20, 20]</t>
+          <t>[20, 20, 20]</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>[69, 60, 76, 85]</t>
+          <t>[60, 76, 85]</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>[69.75, 60.019999999999996, 76.11999999999999, 84.84]</t>
+          <t>[60.019999999999996, 76.11999999999999, 84.84]</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>[67.74, 58.68, 64.05, 73.11]</t>
+          <t>[58.68, 64.05, 73.11]</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>[26.4, 22.63, 33.45, 37.05]</t>
+          <t>[22.63, 33.45, 37.05]</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>[133.91, 157.23, 151.28, 185.27]</t>
+          <t>[157.23, 151.28, 185.27]</t>
         </is>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>[6251.3, 5854.74, 9522.56, 10884.14]</t>
+          <t>[5854.74, 9522.56, 10884.14]</t>
         </is>
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>[6.76, 6.76, 6.76, 6.76]</t>
+          <t>[6.76, 6.76, 6.76]</t>
         </is>
       </c>
     </row>
@@ -6576,52 +6576,52 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>[10, 12, 12, 12, 12]</t>
+          <t>[10, 12, 12, 12]</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>[30, 32, 32, 30, 30]</t>
+          <t>[30, 32, 30, 30]</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 18, 18]</t>
+          <t>[20, 20, 18, 18]</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>[78, 64, 52, 52, 60]</t>
+          <t>[78, 52, 52, 60]</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>[78.47, 64.39, 52.32, 52.309999999999995, 60.019999999999996]</t>
+          <t>[78.47, 52.32, 52.309999999999995, 60.019999999999996]</t>
         </is>
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>[67.07, 60.7, 48.3, 41.58, 56.67]</t>
+          <t>[67.07, 48.3, 41.58, 56.67]</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>[29.08, 23.12, 21.26, 20.51, 24.07]</t>
+          <t>[29.08, 21.26, 20.51, 24.07]</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>[146.41, 145.04, 179.12, 168.12, 180.34]</t>
+          <t>[146.41, 179.12, 168.12, 180.34]</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>[7069.06, 5648.01, 5762.28, 5712.9, 6764.81]</t>
+          <t>[7069.06, 5762.28, 5712.9, 6764.81]</t>
         </is>
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>[5.7, 5.7, 5.7, 5.7, 5.7]</t>
+          <t>[5.7, 5.7, 5.7, 5.7]</t>
         </is>
       </c>
     </row>
@@ -6792,52 +6792,52 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>[10, 12, 10, 10, 12]</t>
+          <t>[12, 10, 10, 12]</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>[20, 18, 20, 20, 18]</t>
+          <t>[18, 20, 20, 18]</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>[77, 68, 81, 71, 68]</t>
+          <t>[68, 81, 71, 68]</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>[77.47, 68.07, 81.83, 71.09, 68.08]</t>
+          <t>[68.07, 81.83, 71.09, 68.08]</t>
         </is>
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>[64.06, 61.37, 72.78, 64.72999999999999, 64.39]</t>
+          <t>[61.37, 72.78, 64.72999999999999, 64.39]</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>[29.24, 28.48, 33.6, 31.59, 30.37]</t>
+          <t>[28.48, 33.6, 31.59, 30.37]</t>
         </is>
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>[141.14, 171.05, 167.78, 181.63, 199.48]</t>
+          <t>[171.05, 167.78, 181.63, 199.48]</t>
         </is>
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>[7644.75, 7998.98, 9571.38, 9160.82, 8819.85]</t>
+          <t>[7998.98, 9571.38, 9160.82, 8819.85]</t>
         </is>
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>[0.31, 0.31, 0.31, 0.31, 0.31]</t>
+          <t>[0.31, 0.31, 0.31, 0.31]</t>
         </is>
       </c>
     </row>
@@ -7296,52 +7296,52 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>[10, 10, 12, 10, 20]</t>
+          <t>[10, 12, 10, 20]</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>[18, 30, 30, 18, 34]</t>
+          <t>[18, 30, 18, 34]</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>[8, 20, 18, 8, 14]</t>
+          <t>[8, 18, 8, 14]</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>[187, 196, 115, 156, 29]</t>
+          <t>[187, 115, 156, 29]</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>[187.47, 195.85000000000002, 115.7, 155.94, 27.5]</t>
+          <t>[187.47, 115.7, 155.94, 27.5]</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>[178.41, 184.11, 94.24000000000001, 136.82, 26.16]</t>
+          <t>[178.41, 94.24000000000001, 136.82, 26.16]</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>[71.22, 84.46, 52.2, 68.88, 10.1]</t>
+          <t>[71.22, 52.2, 68.88, 10.1]</t>
         </is>
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>[92.0, 158.01, 245.18, 165.01, 88.9]</t>
+          <t>[92.0, 245.18, 165.01, 88.9]</t>
         </is>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>[19613.36, 22784.2, 16882.44, 19948.75, 2842.21]</t>
+          <t>[19613.36, 16882.44, 19948.75, 2842.21]</t>
         </is>
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>[-3.57, -3.57, -3.57, -3.57, -3.57]</t>
+          <t>[-3.57, -3.57, -3.57, -3.57]</t>
         </is>
       </c>
     </row>
@@ -7368,52 +7368,52 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>[10, 12, 12, 12, 10]</t>
+          <t>[12, 12, 12, 10]</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>[18, 30, 32, 32, 30]</t>
+          <t>[30, 32, 32, 30]</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>[8, 18, 20, 20, 20]</t>
+          <t>[18, 20, 20, 20]</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>[166, 45, 75, 138, 194]</t>
+          <t>[45, 75, 138, 194]</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>[166.34, 45.269999999999996, 75.79, 138.84, 194.17]</t>
+          <t>[45.269999999999996, 75.79, 138.84, 194.17]</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>[149.24, 40.58, 75.45, 120.73, 184.77999999999997]</t>
+          <t>[40.58, 75.45, 120.73, 184.77999999999997]</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>[74.14, 18.72, 28.69, 54.33, 86.22]</t>
+          <t>[18.72, 28.69, 54.33, 86.22]</t>
         </is>
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>[179.88, 175.18, 198.79, 173.78, 166.52]</t>
+          <t>[175.18, 198.79, 173.78, 166.52]</t>
         </is>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>[23304.64, 5127.07, 8338.86, 15526.18, 23448.15]</t>
+          <t>[5127.07, 8338.86, 15526.18, 23448.15]</t>
         </is>
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>[0.38, 0.38, 0.38, 0.38, 0.38]</t>
+          <t>[0.38, 0.38, 0.38, 0.38]</t>
         </is>
       </c>
     </row>
@@ -7512,52 +7512,52 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>[10, 12, 12, 10, 10]</t>
+          <t>[12, 12, 10, 10]</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>[30, 32, 30, 30, 30]</t>
+          <t>[32, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>[20, 20, 18, 20, 20]</t>
+          <t>[20, 18, 20, 20]</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>[189, 104, 68, 193, 161]</t>
+          <t>[104, 68, 193, 161]</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>[189.47, 103.96, 67.41, 193.5, 161.64]</t>
+          <t>[103.96, 67.41, 193.5, 161.64]</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
         <is>
-          <t>[169.02, 98.25999999999999, 65.39999999999999, 155.94, 146.22]</t>
+          <t>[98.25999999999999, 65.39999999999999, 155.94, 146.22]</t>
         </is>
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>[75.77, 43.14, 30.57, 87.33, 70.7]</t>
+          <t>[43.14, 30.57, 87.33, 70.7]</t>
         </is>
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>[109.75, 160.68, 184.11, 169.69, 172.83]</t>
+          <t>[160.68, 184.11, 169.69, 172.83]</t>
         </is>
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>[17991.3, 11977.23, 9421.63, 23195.48, 19329.84]</t>
+          <t>[11977.23, 9421.63, 23195.48, 19329.84]</t>
         </is>
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>[-6.55, -6.55, -6.55, -6.55, -6.55]</t>
+          <t>[-6.55, -6.55, -6.55, -6.55]</t>
         </is>
       </c>
     </row>
@@ -8016,52 +8016,52 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>[12, 12, 10, 12]</t>
+          <t>[12, 10, 12]</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>[18, 18, 20, 18]</t>
+          <t>[18, 20, 18]</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>[99, 153, 162, 95]</t>
+          <t>[153, 162, 95]</t>
         </is>
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>[99.6, 153.25, 162.65, 95.24]</t>
+          <t>[153.25, 162.65, 95.24]</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>[85.52, 150.91, 149.91, 79.81]</t>
+          <t>[150.91, 149.91, 79.81]</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>[37.41, 70.22, 71.47, 35.92]</t>
+          <t>[70.22, 71.47, 35.92]</t>
         </is>
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>[109.56, 205.21, 186.07, 164.51]</t>
+          <t>[205.21, 186.07, 164.51]</t>
         </is>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>[8039.66, 21099.7, 19627.3, 9221.45]</t>
+          <t>[21099.7, 19627.3, 9221.45]</t>
         </is>
       </c>
       <c r="N106" t="inlineStr">
         <is>
-          <t>[9.33, 9.33, 9.33, 9.33]</t>
+          <t>[9.33, 9.33, 9.33]</t>
         </is>
       </c>
     </row>
@@ -8160,52 +8160,52 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>[12, 14, 14, 10]</t>
+          <t>[14, 14, 10]</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>[18, 16, 16, 20]</t>
+          <t>[16, 16, 20]</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>[148, 32, 32, 136]</t>
+          <t>[32, 32, 136]</t>
         </is>
       </c>
       <c r="I108" t="inlineStr">
         <is>
-          <t>[148.9, 32.87, 32.53, 135.49]</t>
+          <t>[32.87, 32.53, 135.49]</t>
         </is>
       </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>[123.07, 31.529999999999998, 30.520000000000003, 130.12]</t>
+          <t>[31.529999999999998, 30.520000000000003, 130.12]</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
         <is>
-          <t>[66.52, 12.02, 10.2, 57.85]</t>
+          <t>[12.02, 10.2, 57.85]</t>
         </is>
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>[188.69, 428.82, 72.9, 137.73]</t>
+          <t>[428.82, 72.9, 137.73]</t>
         </is>
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>[19210.15, 3898.67, 2561.02, 15206.32]</t>
+          <t>[3898.67, 2561.02, 15206.32]</t>
         </is>
       </c>
       <c r="N108" t="inlineStr">
         <is>
-          <t>[17.73, 17.73, 17.73, 17.73]</t>
+          <t>[17.73, 17.73, 17.73]</t>
         </is>
       </c>
     </row>
@@ -8376,52 +8376,52 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>[12, 10, 10, 10, 14]</t>
+          <t>[10, 10, 14]</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 32]</t>
+          <t>[30, 30, 32]</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>[18, 20, 20, 20, 18]</t>
+          <t>[20, 20, 18]</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>[73, 100, 105, 108, 32]</t>
+          <t>[105, 108, 32]</t>
         </is>
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>[72.77, 99.92999999999999, 105.3, 108.66, 32.529999999999994]</t>
+          <t>[105.3, 108.66, 32.529999999999994]</t>
         </is>
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>[70.76, 86.52, 101.28, 85.17999999999999, 31.529999999999998]</t>
+          <t>[101.28, 85.17999999999999, 31.529999999999998]</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>[29.44, 39.66, 41.64, 43.68, 12.33]</t>
+          <t>[41.64, 43.68, 12.33]</t>
         </is>
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>[149.02, 131.04, 124.96, 134.87, 333.81]</t>
+          <t>[124.96, 134.87, 333.81]</t>
         </is>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>[8502.52, 10960.5, 10382.81, 11353.94, 4118.1]</t>
+          <t>[10382.81, 11353.94, 4118.1]</t>
         </is>
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>[-1.08, -1.08, -1.08, -1.08, -1.08]</t>
+          <t>[-1.08, -1.08, -1.08]</t>
         </is>
       </c>
     </row>
@@ -8592,52 +8592,52 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>[10, 12, 12, 12, 12]</t>
+          <t>[12, 12, 12, 12]</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 32]</t>
+          <t>[30, 30, 30, 32]</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>[20, 18, 18, 18, 20]</t>
+          <t>[18, 18, 18, 20]</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>[91, 60, 96, 113, 95]</t>
+          <t>[60, 96, 113, 95]</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
         <is>
-          <t>[91.55, 60.36, 96.24, 113.69, 95.24]</t>
+          <t>[60.36, 96.24, 113.69, 95.24]</t>
         </is>
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>[88.86999999999999, 52.98, 82.5, 111.00999999999999, 85.50999999999999]</t>
+          <t>[52.98, 82.5, 111.00999999999999, 85.50999999999999]</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>[37.0, 21.89, 38.22, 44.87, 40.84]</t>
+          <t>[21.89, 38.22, 44.87, 40.84]</t>
         </is>
       </c>
       <c r="L114" t="inlineStr">
         <is>
-          <t>[166.55, 95.15, 128.2, 120.23, 196.17]</t>
+          <t>[95.15, 128.2, 120.23, 196.17]</t>
         </is>
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>[10562.97, 5686.73, 9917.21, 11257.71, 14328.3]</t>
+          <t>[5686.73, 9917.21, 11257.71, 14328.3]</t>
         </is>
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>[-2.17, -2.17, -2.17, -2.17, -2.17]</t>
+          <t>[-2.17, -2.17, -2.17, -2.17]</t>
         </is>
       </c>
     </row>
@@ -9240,52 +9240,52 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>[12, 12, 12, 12, 12]</t>
+          <t>[12, 12, 12, 12]</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>[18, 18, 18, 18, 18]</t>
+          <t>[18, 18, 18, 18]</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>[61, 22, 69, 80, 91]</t>
+          <t>[61, 69, 80, 91]</t>
         </is>
       </c>
       <c r="I123" t="inlineStr">
         <is>
-          <t>[61.37, 22.47, 69.08, 80.82, 91.55]</t>
+          <t>[61.37, 69.08, 80.82, 91.55]</t>
         </is>
       </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>[53.66, 22.47, 63.04, 73.11, 74.78999999999999]</t>
+          <t>[53.66, 63.04, 73.11, 74.78999999999999]</t>
         </is>
       </c>
       <c r="K123" t="inlineStr">
         <is>
-          <t>[24.11, 11.09, 26.23, 31.48, 37.05]</t>
+          <t>[24.11, 26.23, 31.48, 37.05]</t>
         </is>
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>[158.55, 409.01, 137.12, 165.0, 128.87]</t>
+          <t>[158.55, 137.12, 165.0, 128.87]</t>
         </is>
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>[7505.73, 3791.77, 7027.84, 8914.82, 10543.41]</t>
+          <t>[7505.73, 7027.84, 8914.82, 10543.41]</t>
         </is>
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>[22.39, 22.39, 22.39, 22.39, 22.39]</t>
+          <t>[22.39, 22.39, 22.39, 22.39]</t>
         </is>
       </c>
     </row>
@@ -9744,52 +9744,52 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>[12, 10, 10, 12]</t>
+          <t>[10, 10, 12]</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>[18, 20, 20, 18]</t>
+          <t>[20, 20, 18]</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>[179, 172, 163, 157]</t>
+          <t>[172, 163, 157]</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>[179.08, 172.71, 163.65, 157.60999999999999]</t>
+          <t>[172.71, 163.65, 157.60999999999999]</t>
         </is>
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>[151.58, 169.02, 149.56, 139.51]</t>
+          <t>[169.02, 149.56, 139.51]</t>
         </is>
       </c>
       <c r="K130" t="inlineStr">
         <is>
-          <t>[59.17, 57.25, 50.82, 50.89]</t>
+          <t>[57.25, 50.82, 50.89]</t>
         </is>
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>[63.68, 64.2, 60.69, 61.19]</t>
+          <t>[64.2, 60.69, 61.19]</t>
         </is>
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>[12669.44, 13054.44, 11658.27, 11255.22]</t>
+          <t>[13054.44, 11658.27, 11255.22]</t>
         </is>
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>[30.27, 30.27, 30.27, 30.27]</t>
+          <t>[30.27, 30.27, 30.27]</t>
         </is>
       </c>
     </row>
@@ -10104,52 +10104,52 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 10]</t>
+          <t>[10, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>[52, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>[42, 20, 20, 20, 20]</t>
+          <t>[20, 20, 20, 20]</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>[250, 202, 248, 233, 227]</t>
+          <t>[202, 248, 233, 227]</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
         <is>
-          <t>[240.45, 201.89000000000001, 248.5, 233.74, 226.7]</t>
+          <t>[201.89000000000001, 248.5, 233.74, 226.7]</t>
         </is>
       </c>
       <c r="J135" t="inlineStr">
         <is>
-          <t>[243.79999999999998, 188.81, 234.08, 217.98000000000002, 184.11]</t>
+          <t>[188.81, 234.08, 217.98000000000002, 184.11]</t>
         </is>
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>[104.31, 76.23, 91.73, 82.61, 77.61]</t>
+          <t>[76.23, 91.73, 82.61, 77.61]</t>
         </is>
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>[84.56, 85.51, 74.01, 74.36, 67.06]</t>
+          <t>[85.51, 74.01, 74.36, 67.06]</t>
         </is>
       </c>
       <c r="M135" t="inlineStr">
         <is>
-          <t>[18511.76, 16399.61, 18700.85, 16424.85, 15218.08]</t>
+          <t>[16399.61, 18700.85, 16424.85, 15218.08]</t>
         </is>
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>[8.65, 8.65, 8.65, 8.65, 8.65]</t>
+          <t>[8.65, 8.65, 8.65, 8.65]</t>
         </is>
       </c>
     </row>
@@ -10176,52 +10176,52 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 10]</t>
+          <t>[10, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>[32, 32, 30, 30, 30]</t>
+          <t>[32, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>[22, 22, 20, 20, 20]</t>
+          <t>[22, 20, 20, 20]</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>[230, 207, 222, 200, 206]</t>
+          <t>[207, 222, 200, 206]</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>[229.39000000000001, 206.91, 222.34, 200.54, 205.91]</t>
+          <t>[206.91, 222.34, 200.54, 205.91]</t>
         </is>
       </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>[228.05, 202.22, 203.56, 167.34, 165.67000000000002]</t>
+          <t>[202.22, 203.56, 167.34, 165.67000000000002]</t>
         </is>
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>[83.41, 73.57, 75.08, 66.8, 72.6]</t>
+          <t>[73.57, 75.08, 66.8, 72.6]</t>
         </is>
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>[81.73, 75.3, 56.94, 61.06, 63.97]</t>
+          <t>[75.3, 56.94, 61.06, 63.97]</t>
         </is>
       </c>
       <c r="M136" t="inlineStr">
         <is>
-          <t>[16967.87, 15727.72, 14376.51, 13615.12, 14590.26]</t>
+          <t>[15727.72, 14376.51, 13615.12, 14590.26]</t>
         </is>
       </c>
       <c r="N136" t="inlineStr">
         <is>
-          <t>[13.83, 13.83, 13.83, 13.83, 13.83]</t>
+          <t>[13.83, 13.83, 13.83, 13.83]</t>
         </is>
       </c>
     </row>
@@ -10248,52 +10248,52 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 10]</t>
+          <t>[10, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>[52, 30, 30, 32, 30]</t>
+          <t>[30, 30, 32, 30]</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>[42, 20, 20, 22, 20]</t>
+          <t>[20, 20, 22, 20]</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>[240, 186, 199, 228, 219]</t>
+          <t>[186, 199, 228, 219]</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
         <is>
-          <t>[224.69, 186.12, 199.2, 228.37, 219.65]</t>
+          <t>[186.12, 199.2, 228.37, 219.65]</t>
         </is>
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>[221.0, 152.25, 177.07, 195.84, 184.11]</t>
+          <t>[152.25, 177.07, 195.84, 184.11]</t>
         </is>
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>[105.92, 62.79, 65.25, 77.45, 72.98]</t>
+          <t>[62.79, 65.25, 77.45, 72.98]</t>
         </is>
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>[92.1, 64.47, 56.63, 61.56, 63.92]</t>
+          <t>[64.47, 56.63, 61.56, 63.92]</t>
         </is>
       </c>
       <c r="M137" t="inlineStr">
         <is>
-          <t>[20429.08, 13981.08, 13529.9, 14898.97, 15395.99]</t>
+          <t>[13981.08, 13529.9, 14898.97, 15395.99]</t>
         </is>
       </c>
       <c r="N137" t="inlineStr">
         <is>
-          <t>[11.26, 11.26, 11.26, 11.26, 11.26]</t>
+          <t>[11.26, 11.26, 11.26, 11.26]</t>
         </is>
       </c>
     </row>
@@ -11616,52 +11616,52 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>[12, 12, 12, 12]</t>
+          <t>[12, 12, 12]</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>[32, 32, 34, 32]</t>
+          <t>[32, 34, 32]</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>[20, 20, 22, 20]</t>
+          <t>[20, 22, 20]</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>[117, 144, 82, 130]</t>
+          <t>[144, 82, 130]</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>[117.71, 144.54, 81.83, 129.78]</t>
+          <t>[144.54, 81.83, 129.78]</t>
         </is>
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>[102.28, 132.47, 81.83, 128.11]</t>
+          <t>[132.47, 81.83, 128.11]</t>
         </is>
       </c>
       <c r="K156" t="inlineStr">
         <is>
-          <t>[46.78, 52.64, 34.07, 48.72]</t>
+          <t>[52.64, 34.07, 48.72]</t>
         </is>
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>[154.33, 182.04, 145.3, 175.66]</t>
+          <t>[182.04, 145.3, 175.66]</t>
         </is>
       </c>
       <c r="M156" t="inlineStr">
         <is>
-          <t>[11675.64, 12716.85, 8589.51, 12302.53]</t>
+          <t>[12716.85, 8589.51, 12302.53]</t>
         </is>
       </c>
       <c r="N156" t="inlineStr">
         <is>
-          <t>[13.09, 13.09, 13.09, 13.09]</t>
+          <t>[13.09, 13.09, 13.09]</t>
         </is>
       </c>
     </row>
@@ -11688,52 +11688,52 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>[12, 12, 12, 12]</t>
+          <t>[12, 12]</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>[20, 32, 30, 20]</t>
+          <t>[30, 20]</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>[8, 20, 18, 8]</t>
+          <t>[18, 8]</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
         <is>
-          <t>[119, 162, 58, 77]</t>
+          <t>[58, 77]</t>
         </is>
       </c>
       <c r="I157" t="inlineStr">
         <is>
-          <t>[119.05, 162.65, 58.01, 77.8]</t>
+          <t>[58.01, 77.8]</t>
         </is>
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>[107.64999999999999, 152.92000000000002, 50.64, 70.42]</t>
+          <t>[50.64, 70.42]</t>
         </is>
       </c>
       <c r="K157" t="inlineStr">
         <is>
-          <t>[36.02, 55.15, 25.66, 30.71]</t>
+          <t>[25.66, 30.71]</t>
         </is>
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>[55.45, 78.51, 155.49, 130.5]</t>
+          <t>[155.49, 130.5]</t>
         </is>
       </c>
       <c r="M157" t="inlineStr">
         <is>
-          <t>[6416.58, 9443.9, 6755.93, 8612.3]</t>
+          <t>[6755.93, 8612.3]</t>
         </is>
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>[8.59, 8.59, 8.59, 8.59]</t>
+          <t>[8.59, 8.59]</t>
         </is>
       </c>
     </row>
@@ -12048,52 +12048,52 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>[12, 12, 12, 12, 12]</t>
+          <t>[12, 12, 12, 12]</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>[32, 32, 32, 20, 20]</t>
+          <t>[32, 32, 20, 20]</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 8, 8]</t>
+          <t>[20, 20, 8, 8]</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
         <is>
-          <t>[132, 155, 146, 64, 59]</t>
+          <t>[155, 146, 64, 59]</t>
         </is>
       </c>
       <c r="I162" t="inlineStr">
         <is>
-          <t>[131.8, 155.61, 146.89, 64.05, 59.36]</t>
+          <t>[155.61, 146.89, 64.05, 59.36]</t>
         </is>
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>[126.77000000000001, 146.22, 138.84, 53.99, 53.66]</t>
+          <t>[146.22, 138.84, 53.99, 53.66]</t>
         </is>
       </c>
       <c r="K162" t="inlineStr">
         <is>
-          <t>[43.27, 61.1, 56.05, 20.62, 19.57]</t>
+          <t>[61.1, 56.05, 20.62, 19.57]</t>
         </is>
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>[58.12, 107.34, 142.4, 82.15, 73.69]</t>
+          <t>[107.34, 142.4, 82.15, 73.69]</t>
         </is>
       </c>
       <c r="M162" t="inlineStr">
         <is>
-          <t>[6541.09, 16532.68, 13128.16, 4960.02, 4595.16]</t>
+          <t>[16532.68, 13128.16, 4960.02, 4595.16]</t>
         </is>
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>[7.16, 7.16, 7.16, 7.16, 7.16]</t>
+          <t>[7.16, 7.16, 7.16, 7.16]</t>
         </is>
       </c>
     </row>
@@ -12480,52 +12480,52 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 10]</t>
+          <t>[10, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 52]</t>
+          <t>[30, 30, 30, 52]</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 20, 42]</t>
+          <t>[20, 20, 20, 42]</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
         <is>
-          <t>[151, 146, 130, 127, 129]</t>
+          <t>[146, 130, 127, 129]</t>
         </is>
       </c>
       <c r="I168" t="inlineStr">
         <is>
-          <t>[151.24, 146.55, 129.78, 127.1, 126.09]</t>
+          <t>[146.55, 129.78, 127.1, 126.09]</t>
         </is>
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>[149.57000000000002, 135.15, 123.74999999999999, 114.69000000000001, 118.38000000000001]</t>
+          <t>[135.15, 123.74999999999999, 114.69000000000001, 118.38000000000001]</t>
         </is>
       </c>
       <c r="K168" t="inlineStr">
         <is>
-          <t>[67.24, 65.02, 60.34, 50.56, 54.52]</t>
+          <t>[65.02, 60.34, 50.56, 54.52]</t>
         </is>
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>[161.43, 132.11, 176.9, 143.13, 147.59]</t>
+          <t>[132.11, 176.9, 143.13, 147.59]</t>
         </is>
       </c>
       <c r="M168" t="inlineStr">
         <is>
-          <t>[19040.48, 17962.94, 17463.6, 13565.81, 12875.94]</t>
+          <t>[17962.94, 17463.6, 13565.81, 12875.94]</t>
         </is>
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>[4.58, 4.58, 4.58, 4.58, 4.58]</t>
+          <t>[4.58, 4.58, 4.58, 4.58]</t>
         </is>
       </c>
     </row>
@@ -12984,52 +12984,52 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>[10, 2, 10, 10, 10]</t>
+          <t>[10, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>[30, 30, 32, 30, 30]</t>
+          <t>[30, 32, 30, 30]</t>
         </is>
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>[20, 28, 22, 20, 20]</t>
+          <t>[20, 22, 20, 20]</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
         <is>
-          <t>[174, 125, 118, 114, 115]</t>
+          <t>[174, 118, 114, 115]</t>
         </is>
       </c>
       <c r="I175" t="inlineStr">
         <is>
-          <t>[174.38, 124.75, 117.38, 114.02, 115.36]</t>
+          <t>[174.38, 117.38, 114.02, 115.36]</t>
         </is>
       </c>
       <c r="J175" t="inlineStr">
         <is>
-          <t>[155.94, 102.96000000000001, 111.34, 103.63000000000001, 115.03]</t>
+          <t>[155.94, 111.34, 103.63000000000001, 115.03]</t>
         </is>
       </c>
       <c r="K175" t="inlineStr">
         <is>
-          <t>[68.75, 55.79, 39.12, 50.28, 47.31]</t>
+          <t>[68.75, 39.12, 50.28, 47.31]</t>
         </is>
       </c>
       <c r="L175" t="inlineStr">
         <is>
-          <t>[127.92, 217.14, 107.46, 141.54, 131.1]</t>
+          <t>[127.92, 107.46, 141.54, 131.1]</t>
         </is>
       </c>
       <c r="M175" t="inlineStr">
         <is>
-          <t>[17405.68, 16321.53, 9854.72, 13746.53, 12975.17]</t>
+          <t>[17405.68, 9854.72, 13746.53, 12975.17]</t>
         </is>
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>[14.05, 14.05, 14.05, 14.05, 14.05]</t>
+          <t>[14.05, 14.05, 14.05, 14.05]</t>
         </is>
       </c>
     </row>
@@ -13056,52 +13056,52 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 52, 32]</t>
+          <t>[30, 52, 32]</t>
         </is>
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 42, 22]</t>
+          <t>[20, 42, 22]</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>[181, 128, 119, 124, 82]</t>
+          <t>[119, 124, 82]</t>
         </is>
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>[181.09, 127.42999999999999, 118.71, 119.05, 81.82]</t>
+          <t>[118.71, 119.05, 81.82]</t>
         </is>
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>[169.69, 122.74, 107.97999999999999, 116.7, 68.41]</t>
+          <t>[107.97999999999999, 116.7, 68.41]</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
         <is>
-          <t>[74.86, 58.49, 51.7, 56.25, 32.23]</t>
+          <t>[51.7, 56.25, 32.23]</t>
         </is>
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>[133.21, 149.72, 170.94, 154.88, 141.18]</t>
+          <t>[170.94, 154.88, 141.18]</t>
         </is>
       </c>
       <c r="M176" t="inlineStr">
         <is>
-          <t>[19145.18, 16260.59, 14876.87, 14273.46, 9296.99]</t>
+          <t>[14876.87, 14273.46, 9296.99]</t>
         </is>
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>[14.44, 14.44, 14.44, 14.44, 14.44]</t>
+          <t>[14.44, 14.44, 14.44]</t>
         </is>
       </c>
     </row>
@@ -13704,52 +13704,52 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>[10, 12, 10, 10, 10]</t>
+          <t>[10, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>[20, 18, 20, 20, 20]</t>
+          <t>[20, 20, 20, 20]</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>[98, 111, 145, 163, 154]</t>
+          <t>[98, 145, 163, 154]</t>
         </is>
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>[97.59, 111.67, 144.87, 163.32, 154.26]</t>
+          <t>[97.59, 144.87, 163.32, 154.26]</t>
         </is>
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>[91.22, 93.56, 130.79, 141.52, 141.85999999999999]</t>
+          <t>[91.22, 130.79, 141.52, 141.85999999999999]</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
         <is>
-          <t>[36.35, 43.18, 65.0, 71.93, 70.07]</t>
+          <t>[36.35, 65.0, 71.93, 70.07]</t>
         </is>
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>[181.17, 162.53, 178.75, 172.28, 183.94]</t>
+          <t>[181.17, 178.75, 172.28, 183.94]</t>
         </is>
       </c>
       <c r="M185" t="inlineStr">
         <is>
-          <t>[10411.53, 12530.3, 20076.79, 21184.66, 21557.21]</t>
+          <t>[10411.53, 20076.79, 21184.66, 21557.21]</t>
         </is>
       </c>
       <c r="N185" t="inlineStr">
         <is>
-          <t>[-15.83, -15.83, -15.83, -15.83, -15.83]</t>
+          <t>[-15.83, -15.83, -15.83, -15.83]</t>
         </is>
       </c>
     </row>
@@ -14064,52 +14064,52 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>[12, 10, 10]</t>
+          <t>[10, 10]</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>[30, 30, 30]</t>
+          <t>[30, 30]</t>
         </is>
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>[18, 20, 20]</t>
+          <t>[20, 20]</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>[90, 112, 86]</t>
+          <t>[112, 86]</t>
         </is>
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>[89.86999999999999, 112.01, 85.85]</t>
+          <t>[112.01, 85.85]</t>
         </is>
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>[78.47, 93.56, 73.45]</t>
+          <t>[93.56, 73.45]</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
         <is>
-          <t>[36.63, 47.08, 34.92]</t>
+          <t>[47.08, 34.92]</t>
         </is>
       </c>
       <c r="L190" t="inlineStr">
         <is>
-          <t>[131.65, 163.71, 231.36]</t>
+          <t>[163.71, 231.36]</t>
         </is>
       </c>
       <c r="M190" t="inlineStr">
         <is>
-          <t>[10569.61, 14711.58, 10541.53]</t>
+          <t>[14711.58, 10541.53]</t>
         </is>
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>[6.76, 6.76, 6.76]</t>
+          <t>[6.76, 6.76]</t>
         </is>
       </c>
     </row>
@@ -14352,52 +14352,52 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>[10, 12, 10, 10, 10]</t>
+          <t>[12, 10, 10, 10]</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 32, 30]</t>
+          <t>[30, 30, 32, 30]</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>[20, 18, 20, 22, 20]</t>
+          <t>[18, 20, 22, 20]</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
         <is>
-          <t>[152, 118, 89, 126, 116]</t>
+          <t>[118, 89, 126, 116]</t>
         </is>
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>[151.91, 118.72, 89.2, 126.43, 116.37]</t>
+          <t>[118.72, 89.2, 126.43, 116.37]</t>
         </is>
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>[140.51, 94.57, 74.45, 119.05000000000001, 103.96]</t>
+          <t>[94.57, 74.45, 119.05000000000001, 103.96]</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
         <is>
-          <t>[65.64, 52.14, 37.28, 56.96, 50.53]</t>
+          <t>[52.14, 37.28, 56.96, 50.53]</t>
         </is>
       </c>
       <c r="L194" t="inlineStr">
         <is>
-          <t>[225.19, 163.28, 186.84, 172.33, 198.27]</t>
+          <t>[163.28, 186.84, 172.33, 198.27]</t>
         </is>
       </c>
       <c r="M194" t="inlineStr">
         <is>
-          <t>[21046.6, 16074.44, 11446.66, 17100.62, 15999.59]</t>
+          <t>[16074.44, 11446.66, 17100.62, 15999.59]</t>
         </is>
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>[5.7, 5.7, 5.7, 5.7, 5.7]</t>
+          <t>[5.7, 5.7, 5.7, 5.7]</t>
         </is>
       </c>
     </row>
@@ -14496,52 +14496,52 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10]</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30]</t>
         </is>
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 20]</t>
+          <t>[20, 20]</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>[135, 79, 123, 129]</t>
+          <t>[123, 129]</t>
         </is>
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>[135.15, 78.47, 122.74, 129.11]</t>
+          <t>[122.74, 129.11]</t>
         </is>
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>[110.67, 70.09, 116.03999999999999, 106.64]</t>
+          <t>[116.03999999999999, 106.64]</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
         <is>
-          <t>[56.74, 30.03, 51.56, 53.36]</t>
+          <t>[51.56, 53.36]</t>
         </is>
       </c>
       <c r="L196" t="inlineStr">
         <is>
-          <t>[185.13, 164.96, 163.6, 150.3]</t>
+          <t>[163.6, 150.3]</t>
         </is>
       </c>
       <c r="M196" t="inlineStr">
         <is>
-          <t>[17135.08, 9011.91, 15439.1, 16061.49]</t>
+          <t>[15439.1, 16061.49]</t>
         </is>
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>[13.77, 13.77, 13.77, 13.77]</t>
+          <t>[13.77, 13.77]</t>
         </is>
       </c>
     </row>
@@ -15216,52 +15216,52 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 20]</t>
+          <t>[20, 20, 20]</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
         <is>
-          <t>[286, 283, 254, 218]</t>
+          <t>[283, 254, 218]</t>
         </is>
       </c>
       <c r="I206" t="inlineStr">
         <is>
-          <t>[285.39, 283.37, 253.53, 218.99]</t>
+          <t>[283.37, 253.53, 218.99]</t>
         </is>
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t>[272.97999999999996, 273.65, 224.01999999999998, 187.8]</t>
+          <t>[273.65, 224.01999999999998, 187.8]</t>
         </is>
       </c>
       <c r="K206" t="inlineStr">
         <is>
-          <t>[83.83, 116.45, 101.26, 86.03]</t>
+          <t>[116.45, 101.26, 86.03]</t>
         </is>
       </c>
       <c r="L206" t="inlineStr">
         <is>
-          <t>[78.96, 195.3, 163.65, 165.13]</t>
+          <t>[195.3, 163.65, 165.13]</t>
         </is>
       </c>
       <c r="M206" t="inlineStr">
         <is>
-          <t>[16632.31, 31652.35, 27681.13, 24131.17]</t>
+          <t>[31652.35, 27681.13, 24131.17]</t>
         </is>
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>[3.66, 3.66, 3.66, 3.66]</t>
+          <t>[3.66, 3.66, 3.66]</t>
         </is>
       </c>
     </row>
@@ -15432,52 +15432,52 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>[18, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>[8, 20, 20, 20]</t>
+          <t>[20, 20, 20]</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
         <is>
-          <t>[285, 265, 300, 257]</t>
+          <t>[265, 300, 257]</t>
         </is>
       </c>
       <c r="I209" t="inlineStr">
         <is>
-          <t>[285.05, 265.6, 300.82, 257.55]</t>
+          <t>[265.6, 300.82, 257.55]</t>
         </is>
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>[270.29, 232.74, 292.77, 241.12]</t>
+          <t>[232.74, 292.77, 241.12]</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
         <is>
-          <t>[123.95, 115.24, 94.29, 110.64]</t>
+          <t>[115.24, 94.29, 110.64]</t>
         </is>
       </c>
       <c r="L209" t="inlineStr">
         <is>
-          <t>[145.41, 173.69, 77.92, 168.76]</t>
+          <t>[173.69, 77.92, 168.76]</t>
         </is>
       </c>
       <c r="M209" t="inlineStr">
         <is>
-          <t>[38403.68, 33647.08, 23469.16, 32087.34]</t>
+          <t>[33647.08, 23469.16, 32087.34]</t>
         </is>
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>[10.32, 10.32, 10.32, 10.32]</t>
+          <t>[10.32, 10.32, 10.32]</t>
         </is>
       </c>
     </row>
@@ -15792,52 +15792,52 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10]</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30]</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 20]</t>
+          <t>[20, 20]</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>[242, 242, 263, 219]</t>
+          <t>[263, 219]</t>
         </is>
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>[241.46, 242.8, 263.26, 218.98]</t>
+          <t>[263.26, 218.98]</t>
         </is>
       </c>
       <c r="J214" t="inlineStr">
         <is>
-          <t>[239.11, 233.08, 242.13, 175.73]</t>
+          <t>[242.13, 175.73]</t>
         </is>
       </c>
       <c r="K214" t="inlineStr">
         <is>
-          <t>[71.1, 106.54, 108.04, 98.7]</t>
+          <t>[108.04, 98.7]</t>
         </is>
       </c>
       <c r="L214" t="inlineStr">
         <is>
-          <t>[71.58, 174.17, 178.41, 179.0]</t>
+          <t>[178.41, 179.0]</t>
         </is>
       </c>
       <c r="M214" t="inlineStr">
         <is>
-          <t>[16364.94, 30711.16, 29055.88, 29605.62]</t>
+          <t>[29055.88, 29605.62]</t>
         </is>
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>[9.33, 9.33, 9.33, 9.33]</t>
+          <t>[9.33, 9.33]</t>
         </is>
       </c>
     </row>
@@ -15936,52 +15936,52 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 20]</t>
+          <t>[20, 20, 20]</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>[232, 290, 214, 211]</t>
+          <t>[232, 214, 211]</t>
         </is>
       </c>
       <c r="I216" t="inlineStr">
         <is>
-          <t>[231.73000000000002, 289.07, 214.96, 211.95]</t>
+          <t>[231.73000000000002, 214.96, 211.95]</t>
         </is>
       </c>
       <c r="J216" t="inlineStr">
         <is>
-          <t>[214.3, 260.91, 193.16, 187.47]</t>
+          <t>[214.3, 193.16, 187.47]</t>
         </is>
       </c>
       <c r="K216" t="inlineStr">
         <is>
-          <t>[97.29, 132.83, 86.27, 89.14]</t>
+          <t>[97.29, 86.27, 89.14]</t>
         </is>
       </c>
       <c r="L216" t="inlineStr">
         <is>
-          <t>[200.81, 197.47, 171.63, 189.58]</t>
+          <t>[200.81, 171.63, 189.58]</t>
         </is>
       </c>
       <c r="M216" t="inlineStr">
         <is>
-          <t>[27488.47, 38435.97, 23435.46, 25555.43]</t>
+          <t>[27488.47, 23435.46, 25555.43]</t>
         </is>
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>[17.73, 17.73, 17.73, 17.73]</t>
+          <t>[17.73, 17.73, 17.73]</t>
         </is>
       </c>
     </row>
@@ -16440,52 +16440,52 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>[12, 12, 12]</t>
+          <t>[12, 12]</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>[34, 30, 30]</t>
+          <t>[30, 30]</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>[22, 18, 18]</t>
+          <t>[18, 18]</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>[69, 78, 90]</t>
+          <t>[78, 90]</t>
         </is>
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>[69.75, 78.47, 90.55]</t>
+          <t>[78.47, 90.55]</t>
         </is>
       </c>
       <c r="J223" t="inlineStr">
         <is>
-          <t>[67.07, 70.09, 84.85]</t>
+          <t>[70.09, 84.85]</t>
         </is>
       </c>
       <c r="K223" t="inlineStr">
         <is>
-          <t>[27.9, 34.86, 39.4]</t>
+          <t>[34.86, 39.4]</t>
         </is>
       </c>
       <c r="L223" t="inlineStr">
         <is>
-          <t>[185.25, 221.39, 230.1]</t>
+          <t>[221.39, 230.1]</t>
         </is>
       </c>
       <c r="M223" t="inlineStr">
         <is>
-          <t>[8540.19, 11013.93, 12580.02]</t>
+          <t>[11013.93, 12580.02]</t>
         </is>
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>[-9.16, -9.16, -9.16]</t>
+          <t>[-9.16, -9.16]</t>
         </is>
       </c>
     </row>
@@ -16800,52 +16800,52 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>[12, 12, 12, 8, 12]</t>
+          <t>[12, 8, 12]</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>[32, 34, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>[20, 22, 18, 22, 18]</t>
+          <t>[18, 22, 18]</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>[59, 70, 79, 20, 80]</t>
+          <t>[79, 20, 80]</t>
         </is>
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>[59.019999999999996, 70.09, 79.14, 19.45, 80.49]</t>
+          <t>[79.14, 19.45, 80.49]</t>
         </is>
       </c>
       <c r="J228" t="inlineStr">
         <is>
-          <t>[54.66, 64.39, 64.39, 16.77, 67.08]</t>
+          <t>[64.39, 16.77, 67.08]</t>
         </is>
       </c>
       <c r="K228" t="inlineStr">
         <is>
-          <t>[23.94, 27.9, 33.67, 7.01, 34.93]</t>
+          <t>[33.67, 7.01, 34.93]</t>
         </is>
       </c>
       <c r="L228" t="inlineStr">
         <is>
-          <t>[225.08, 139.4, 234.67, 137.95, 200.45]</t>
+          <t>[234.67, 137.95, 200.45]</t>
         </is>
       </c>
       <c r="M228" t="inlineStr">
         <is>
-          <t>[7384.88, 8641.32, 11381.11, 2668.05, 10968.06]</t>
+          <t>[11381.11, 2668.05, 10968.06]</t>
         </is>
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>[19.21, 19.21, 19.21, 19.21, 19.21]</t>
+          <t>[19.21, 19.21, 19.21]</t>
         </is>
       </c>
     </row>
@@ -17232,52 +17232,52 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>[12, 22, 10, 12, 12]</t>
+          <t>[22, 10, 12, 12]</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>[32, 38, 30, 34, 32]</t>
+          <t>[38, 30, 34, 32]</t>
         </is>
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>[20, 16, 20, 22, 20]</t>
+          <t>[16, 20, 22, 20]</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>[76, 21, 101, 26, 39]</t>
+          <t>[21, 101, 26, 39]</t>
         </is>
       </c>
       <c r="I234" t="inlineStr">
         <is>
-          <t>[76.8, 21.46, 101.61, 25.82, 39.91]</t>
+          <t>[21.46, 101.61, 25.82, 39.91]</t>
         </is>
       </c>
       <c r="J234" t="inlineStr">
         <is>
-          <t>[65.72999999999999, 20.79, 87.86, 24.82, 34.54]</t>
+          <t>[20.79, 87.86, 24.82, 34.54]</t>
         </is>
       </c>
       <c r="K234" t="inlineStr">
         <is>
-          <t>[33.21, 8.77, 43.68, 8.8, 16.49]</t>
+          <t>[8.77, 43.68, 8.8, 16.49]</t>
         </is>
       </c>
       <c r="L234" t="inlineStr">
         <is>
-          <t>[229.51, 175.32, 205.75, 154.57, 213.56]</t>
+          <t>[175.32, 205.75, 154.57, 213.56]</t>
         </is>
       </c>
       <c r="M234" t="inlineStr">
         <is>
-          <t>[10544.54, 2548.62, 13906.61, 2378.85, 5369.73]</t>
+          <t>[2548.62, 13906.61, 2378.85, 5369.73]</t>
         </is>
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>[18.8, 18.8, 18.8, 18.8, 18.8]</t>
+          <t>[18.8, 18.8, 18.8, 18.8]</t>
         </is>
       </c>
     </row>
@@ -17304,52 +17304,52 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>[12, 12, 12]</t>
+          <t>[12, 12]</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>[32, 32, 30]</t>
+          <t>[32, 30]</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>[20, 20, 18]</t>
+          <t>[20, 18]</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>[94, 85, 53]</t>
+          <t>[94, 53]</t>
         </is>
       </c>
       <c r="I235" t="inlineStr">
         <is>
-          <t>[94.57, 85.85, 53.31999999999999]</t>
+          <t>[94.57, 53.31999999999999]</t>
         </is>
       </c>
       <c r="J235" t="inlineStr">
         <is>
-          <t>[90.88, 81.49, 47.959999999999994]</t>
+          <t>[90.88, 47.959999999999994]</t>
         </is>
       </c>
       <c r="K235" t="inlineStr">
         <is>
-          <t>[38.79, 33.21, 21.01]</t>
+          <t>[38.79, 21.01]</t>
         </is>
       </c>
       <c r="L235" t="inlineStr">
         <is>
-          <t>[193.04, 200.79, 153.09]</t>
+          <t>[193.04, 153.09]</t>
         </is>
       </c>
       <c r="M235" t="inlineStr">
         <is>
-          <t>[11853.4, 9633.85, 6320.93]</t>
+          <t>[11853.4, 6320.93]</t>
         </is>
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>[-0.89, -0.89, -0.89]</t>
+          <t>[-0.89, -0.89]</t>
         </is>
       </c>
     </row>
@@ -17592,52 +17592,52 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>[30, 18, 30, 18]</t>
+          <t>[18, 30, 18]</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>[20, 8, 20, 8]</t>
+          <t>[8, 20, 8]</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
         <is>
-          <t>[186, 194, 214, 188]</t>
+          <t>[194, 214, 188]</t>
         </is>
       </c>
       <c r="I239" t="inlineStr">
         <is>
-          <t>[186.45, 194.84, 214.96, 188.13]</t>
+          <t>[194.84, 214.96, 188.13]</t>
         </is>
       </c>
       <c r="J239" t="inlineStr">
         <is>
-          <t>[158.62, 187.8, 183.78, 172.37]</t>
+          <t>[187.8, 183.78, 172.37]</t>
         </is>
       </c>
       <c r="K239" t="inlineStr">
         <is>
-          <t>[73.03, 73.7, 92.49, 82.1]</t>
+          <t>[73.7, 92.49, 82.1]</t>
         </is>
       </c>
       <c r="L239" t="inlineStr">
         <is>
-          <t>[115.73, 110.91, 179.41, 160.83]</t>
+          <t>[110.91, 179.41, 160.83]</t>
         </is>
       </c>
       <c r="M239" t="inlineStr">
         <is>
-          <t>[18082.17, 20685.63, 25274.7, 25117.3]</t>
+          <t>[20685.63, 25274.7, 25117.3]</t>
         </is>
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>[4.04, 4.04, 4.04, 4.04]</t>
+          <t>[4.04, 4.04, 4.04]</t>
         </is>
       </c>
     </row>
@@ -17952,52 +17952,52 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 20]</t>
+          <t>[20, 20, 20]</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>[151, 186, 158, 195]</t>
+          <t>[186, 158, 195]</t>
         </is>
       </c>
       <c r="I244" t="inlineStr">
         <is>
-          <t>[151.25, 186.46, 158.62, 194.84]</t>
+          <t>[186.46, 158.62, 194.84]</t>
         </is>
       </c>
       <c r="J244" t="inlineStr">
         <is>
-          <t>[134.15, 153.93, 154.6, 173.38]</t>
+          <t>[153.93, 154.6, 173.38]</t>
         </is>
       </c>
       <c r="K244" t="inlineStr">
         <is>
-          <t>[60.96, 74.88, 64.16, 73.45]</t>
+          <t>[74.88, 64.16, 73.45]</t>
         </is>
       </c>
       <c r="L244" t="inlineStr">
         <is>
-          <t>[127.79, 162.87, 135.26, 127.06]</t>
+          <t>[162.87, 135.26, 127.06]</t>
         </is>
       </c>
       <c r="M244" t="inlineStr">
         <is>
-          <t>[15486.55, 19111.89, 16612.08, 18974.37]</t>
+          <t>[19111.89, 16612.08, 18974.37]</t>
         </is>
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>[13.83, 13.83, 13.83, 13.83]</t>
+          <t>[13.83, 13.83, 13.83]</t>
         </is>
       </c>
     </row>
@@ -18312,52 +18312,52 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>[30, 30, 32, 30]</t>
+          <t>[30, 32, 30]</t>
         </is>
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>[20, 20, 22, 20]</t>
+          <t>[20, 22, 20]</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>[207, 216, 141, 185]</t>
+          <t>[216, 141, 185]</t>
         </is>
       </c>
       <c r="I249" t="inlineStr">
         <is>
-          <t>[207.25, 216.29999999999998, 141.52, 185.79]</t>
+          <t>[216.29999999999998, 141.52, 185.79]</t>
         </is>
       </c>
       <c r="J249" t="inlineStr">
         <is>
-          <t>[180.09, 186.12, 140.18, 163.32]</t>
+          <t>[186.12, 140.18, 163.32]</t>
         </is>
       </c>
       <c r="K249" t="inlineStr">
         <is>
-          <t>[81.41, 85.44, 58.2, 80.89]</t>
+          <t>[85.44, 58.2, 80.89]</t>
         </is>
       </c>
       <c r="L249" t="inlineStr">
         <is>
-          <t>[138.37, 138.56, 157.84, 243.25]</t>
+          <t>[138.56, 157.84, 243.25]</t>
         </is>
       </c>
       <c r="M249" t="inlineStr">
         <is>
-          <t>[20806.63, 21028.34, 15009.1, 23057.39]</t>
+          <t>[21028.34, 15009.1, 23057.39]</t>
         </is>
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>[9.24, 9.24, 9.24, 9.24]</t>
+          <t>[9.24, 9.24, 9.24]</t>
         </is>
       </c>
     </row>
@@ -18384,52 +18384,52 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 20]</t>
+          <t>[20, 20, 20]</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>[161, 219, 180, 191]</t>
+          <t>[219, 180, 191]</t>
         </is>
       </c>
       <c r="I250" t="inlineStr">
         <is>
-          <t>[161.31, 219.99, 180.09, 191.49]</t>
+          <t>[219.99, 180.09, 191.49]</t>
         </is>
       </c>
       <c r="J250" t="inlineStr">
         <is>
-          <t>[151.25, 180.08, 160.3, 159.97]</t>
+          <t>[180.08, 160.3, 159.97]</t>
         </is>
       </c>
       <c r="K250" t="inlineStr">
         <is>
-          <t>[61.07, 86.9, 78.39, 75.38]</t>
+          <t>[86.9, 78.39, 75.38]</t>
         </is>
       </c>
       <c r="L250" t="inlineStr">
         <is>
-          <t>[112.91, 143.64, 188.9, 166.79]</t>
+          <t>[143.64, 188.9, 166.79]</t>
         </is>
       </c>
       <c r="M250" t="inlineStr">
         <is>
-          <t>[14711.15, 22313.25, 22689.58, 21228.75]</t>
+          <t>[22313.25, 22689.58, 21228.75]</t>
         </is>
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>[9.73, 9.73, 9.73, 9.73]</t>
+          <t>[9.73, 9.73, 9.73]</t>
         </is>
       </c>
     </row>
@@ -18744,52 +18744,52 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>[10, 6, 12, 10, 10]</t>
+          <t>[6, 12, 10, 10]</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 18, 18]</t>
+          <t>[30, 30, 18, 18]</t>
         </is>
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>[20, 24, 18, 8, 8]</t>
+          <t>[24, 18, 8, 8]</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
         <is>
-          <t>[194, 137, 87, 157, 155]</t>
+          <t>[137, 87, 157, 155]</t>
         </is>
       </c>
       <c r="I255" t="inlineStr">
         <is>
-          <t>[193.5, 136.82, 87.52, 157.28, 155.6]</t>
+          <t>[136.82, 87.52, 157.28, 155.6]</t>
         </is>
       </c>
       <c r="J255" t="inlineStr">
         <is>
-          <t>[187.13, 129.79000000000002, 86.17999999999999, 139.51, 154.93]</t>
+          <t>[129.79000000000002, 86.17999999999999, 139.51, 154.93]</t>
         </is>
       </c>
       <c r="K255" t="inlineStr">
         <is>
-          <t>[68.46, 51.11, 27.15, 46.97, 51.83]</t>
+          <t>[51.11, 27.15, 46.97, 51.83]</t>
         </is>
       </c>
       <c r="L255" t="inlineStr">
         <is>
-          <t>[57.86, 165.38, 61.8, 33.49, 51.24]</t>
+          <t>[165.38, 61.8, 33.49, 51.24]</t>
         </is>
       </c>
       <c r="M255" t="inlineStr">
         <is>
-          <t>[13061.14, 14111.92, 6862.22, 10032.7, 13137.35]</t>
+          <t>[14111.92, 6862.22, 10032.7, 13137.35]</t>
         </is>
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>[-1.18, -1.18, -1.18, -1.18, -1.18]</t>
+          <t>[-1.18, -1.18, -1.18, -1.18]</t>
         </is>
       </c>
     </row>
@@ -19032,52 +19032,52 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>[10, 10, 12, 8, 10]</t>
+          <t>[12, 8, 10]</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>[30, 32, 30, 18, 30]</t>
+          <t>[30, 18, 30]</t>
         </is>
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>[20, 22, 18, 10, 20]</t>
+          <t>[18, 10, 20]</t>
         </is>
       </c>
       <c r="H259" t="inlineStr">
         <is>
-          <t>[181, 179, 54, 149, 150]</t>
+          <t>[54, 149, 150]</t>
         </is>
       </c>
       <c r="I259" t="inlineStr">
         <is>
-          <t>[181.43, 179.08, 54.66, 148.89, 150.24]</t>
+          <t>[54.66, 148.89, 150.24]</t>
         </is>
       </c>
       <c r="J259" t="inlineStr">
         <is>
-          <t>[161.31, 177.74, 52.309999999999995, 148.89, 122.74000000000001]</t>
+          <t>[52.309999999999995, 148.89, 122.74000000000001]</t>
         </is>
       </c>
       <c r="K259" t="inlineStr">
         <is>
-          <t>[52.99, 55.05, 22.58, 41.3, 46.31]</t>
+          <t>[22.58, 41.3, 46.31]</t>
         </is>
       </c>
       <c r="L259" t="inlineStr">
         <is>
-          <t>[53.53, 61.68, 182.6, 41.02, 65.36]</t>
+          <t>[182.6, 41.02, 65.36]</t>
         </is>
       </c>
       <c r="M259" t="inlineStr">
         <is>
-          <t>[9890.52, 10153.22, 6157.85, 7236.2, 9725.41]</t>
+          <t>[6157.85, 7236.2, 9725.41]</t>
         </is>
       </c>
       <c r="N259" t="inlineStr">
         <is>
-          <t>[10.85, 10.85, 10.85, 10.85, 10.85]</t>
+          <t>[10.85, 10.85, 10.85]</t>
         </is>
       </c>
     </row>
@@ -19104,52 +19104,52 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>[30, 28, 30, 30]</t>
+          <t>[28, 30, 30]</t>
         </is>
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>[20, 18, 20, 20]</t>
+          <t>[18, 20, 20]</t>
         </is>
       </c>
       <c r="H260" t="inlineStr">
         <is>
-          <t>[159, 137, 171, 165]</t>
+          <t>[137, 171, 165]</t>
         </is>
       </c>
       <c r="I260" t="inlineStr">
         <is>
-          <t>[158.96, 137.49, 171.37, 165.33]</t>
+          <t>[137.49, 171.37, 165.33]</t>
         </is>
       </c>
       <c r="J260" t="inlineStr">
         <is>
-          <t>[147.89, 134.48000000000002, 171.37, 142.86]</t>
+          <t>[134.48000000000002, 171.37, 142.86]</t>
         </is>
       </c>
       <c r="K260" t="inlineStr">
         <is>
-          <t>[50.34, 43.49, 45.22, 47.57]</t>
+          <t>[43.49, 45.22, 47.57]</t>
         </is>
       </c>
       <c r="L260" t="inlineStr">
         <is>
-          <t>[62.94, 64.04, 22.48, 31.21]</t>
+          <t>[64.04, 22.48, 31.21]</t>
         </is>
       </c>
       <c r="M260" t="inlineStr">
         <is>
-          <t>[10621.46, 10739.41, 3651.5, 7742.97]</t>
+          <t>[10739.41, 3651.5, 7742.97]</t>
         </is>
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>[10.3, 10.3, 10.3, 10.3]</t>
+          <t>[10.3, 10.3, 10.3]</t>
         </is>
       </c>
     </row>
@@ -19248,52 +19248,52 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>[10, 10, 8, 12]</t>
+          <t>[10, 8, 12]</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>[32, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>[22, 20, 22, 18]</t>
+          <t>[20, 22, 18]</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
         <is>
-          <t>[177, 182, 69, 91]</t>
+          <t>[182, 69, 91]</t>
         </is>
       </c>
       <c r="I262" t="inlineStr">
         <is>
-          <t>[177.74, 181.42000000000002, 68.07, 91.21]</t>
+          <t>[181.42000000000002, 68.07, 91.21]</t>
         </is>
       </c>
       <c r="J262" t="inlineStr">
         <is>
-          <t>[158.29000000000002, 164.32, 68.07, 82.83]</t>
+          <t>[164.32, 68.07, 82.83]</t>
         </is>
       </c>
       <c r="K262" t="inlineStr">
         <is>
-          <t>[51.9, 54.63, 25.9, 30.17]</t>
+          <t>[54.63, 25.9, 30.17]</t>
         </is>
       </c>
       <c r="L262" t="inlineStr">
         <is>
-          <t>[41.4, 57.16, 199.29, 126.72]</t>
+          <t>[57.16, 199.29, 126.72]</t>
         </is>
       </c>
       <c r="M262" t="inlineStr">
         <is>
-          <t>[7363.74, 11226.56, 8055.72, 7984.34]</t>
+          <t>[11226.56, 8055.72, 7984.34]</t>
         </is>
       </c>
       <c r="N262" t="inlineStr">
         <is>
-          <t>[12.23, 12.23, 12.23, 12.23]</t>
+          <t>[12.23, 12.23, 12.23]</t>
         </is>
       </c>
     </row>
@@ -20112,52 +20112,52 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>[6, 6, 6, 12, 12]</t>
+          <t>[6, 6, 12, 12]</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>[24, 24, 24, 18, 18]</t>
+          <t>[24, 24, 18, 18]</t>
         </is>
       </c>
       <c r="H274" t="inlineStr">
         <is>
-          <t>[85, 82, 105, 96, 87]</t>
+          <t>[82, 105, 96, 87]</t>
         </is>
       </c>
       <c r="I274" t="inlineStr">
         <is>
-          <t>[83.84, 82.49, 104.63, 96.58, 87.19]</t>
+          <t>[82.49, 104.63, 96.58, 87.19]</t>
         </is>
       </c>
       <c r="J274" t="inlineStr">
         <is>
-          <t>[78.14, 81.82, 96.25, 86.86, 80.82000000000001]</t>
+          <t>[81.82, 96.25, 86.86, 80.82000000000001]</t>
         </is>
       </c>
       <c r="K274" t="inlineStr">
         <is>
-          <t>[29.88, 29.51, 38.92, 37.18, 32.16]</t>
+          <t>[29.51, 38.92, 37.18, 32.16]</t>
         </is>
       </c>
       <c r="L274" t="inlineStr">
         <is>
-          <t>[118.97, 122.64, 122.02, 128.8, 126.38]</t>
+          <t>[122.64, 122.02, 128.8, 126.38]</t>
         </is>
       </c>
       <c r="M274" t="inlineStr">
         <is>
-          <t>[6572.26, 6786.33, 9049.53, 8622.8, 7626.38]</t>
+          <t>[6786.33, 9049.53, 8622.8, 7626.38]</t>
         </is>
       </c>
       <c r="N274" t="inlineStr">
         <is>
-          <t>[36.17, 36.17, 36.17, 36.17, 36.17]</t>
+          <t>[36.17, 36.17, 36.17, 36.17]</t>
         </is>
       </c>
     </row>
@@ -20400,52 +20400,52 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>[30, 30, 32, 32, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>[20, 20, 22, 22, 20]</t>
+          <t>[20, 20, 20]</t>
         </is>
       </c>
       <c r="H278" t="inlineStr">
         <is>
-          <t>[121, 139, 154, 145, 130]</t>
+          <t>[121, 139, 130]</t>
         </is>
       </c>
       <c r="I278" t="inlineStr">
         <is>
-          <t>[120.72, 139.17, 154.6, 145.88, 130.12]</t>
+          <t>[120.72, 139.17, 130.12]</t>
         </is>
       </c>
       <c r="J278" t="inlineStr">
         <is>
-          <t>[99.94, 138.84, 135.15, 142.85999999999999, 115.03]</t>
+          <t>[99.94, 138.84, 115.03]</t>
         </is>
       </c>
       <c r="K278" t="inlineStr">
         <is>
-          <t>[45.77, 51.38, 59.75, 57.41, 49.68]</t>
+          <t>[45.77, 51.38, 49.68]</t>
         </is>
       </c>
       <c r="L278" t="inlineStr">
         <is>
-          <t>[114.2, 104.68, 120.73, 118.63, 135.8]</t>
+          <t>[114.2, 104.68, 135.8]</t>
         </is>
       </c>
       <c r="M278" t="inlineStr">
         <is>
-          <t>[10102.37, 11336.15, 14136.22, 12801.13, 11180.77]</t>
+          <t>[10102.37, 11336.15, 11180.77]</t>
         </is>
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>[1.33, 1.33, 1.33, 1.33, 1.33]</t>
+          <t>[1.33, 1.33, 1.33]</t>
         </is>
       </c>
     </row>
@@ -20544,52 +20544,52 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 20]</t>
+          <t>[20, 20, 20]</t>
         </is>
       </c>
       <c r="H280" t="inlineStr">
         <is>
-          <t>[121, 122, 116, 109]</t>
+          <t>[122, 116, 109]</t>
         </is>
       </c>
       <c r="I280" t="inlineStr">
         <is>
-          <t>[121.06, 121.72999999999999, 116.03, 109.33]</t>
+          <t>[121.72999999999999, 116.03, 109.33]</t>
         </is>
       </c>
       <c r="J280" t="inlineStr">
         <is>
-          <t>[98.92999999999999, 119.05, 112.68, 106.31]</t>
+          <t>[119.05, 112.68, 106.31]</t>
         </is>
       </c>
       <c r="K280" t="inlineStr">
         <is>
-          <t>[43.57, 46.09, 45.58, 40.07]</t>
+          <t>[46.09, 45.58, 40.07]</t>
         </is>
       </c>
       <c r="L280" t="inlineStr">
         <is>
-          <t>[99.75, 114.57, 134.49, 106.47]</t>
+          <t>[114.57, 134.49, 106.47]</t>
         </is>
       </c>
       <c r="M280" t="inlineStr">
         <is>
-          <t>[9522.43, 10203.86, 10710.09, 8624.03]</t>
+          <t>[10203.86, 10710.09, 8624.03]</t>
         </is>
       </c>
       <c r="N280" t="inlineStr">
         <is>
-          <t>[14.99, 14.99, 14.99, 14.99]</t>
+          <t>[14.99, 14.99, 14.99]</t>
         </is>
       </c>
     </row>
@@ -20616,52 +20616,52 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>[10, 12, 12]</t>
+          <t>[12, 12]</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>[30, 30, 30]</t>
+          <t>[30, 30]</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>[20, 18, 18]</t>
+          <t>[18, 18]</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
         <is>
-          <t>[124, 123, 112]</t>
+          <t>[123, 112]</t>
         </is>
       </c>
       <c r="I281" t="inlineStr">
         <is>
-          <t>[124.08, 123.75, 112.34]</t>
+          <t>[123.75, 112.34]</t>
         </is>
       </c>
       <c r="J281" t="inlineStr">
         <is>
-          <t>[112.35, 99.27, 86.18]</t>
+          <t>[99.27, 86.18]</t>
         </is>
       </c>
       <c r="K281" t="inlineStr">
         <is>
-          <t>[45.27, 46.31, 43.54]</t>
+          <t>[46.31, 43.54]</t>
         </is>
       </c>
       <c r="L281" t="inlineStr">
         <is>
-          <t>[117.64, 108.93, 118.84]</t>
+          <t>[108.93, 118.84]</t>
         </is>
       </c>
       <c r="M281" t="inlineStr">
         <is>
-          <t>[10109.78, 10446.94, 10319.51]</t>
+          <t>[10446.94, 10319.51]</t>
         </is>
       </c>
       <c r="N281" t="inlineStr">
         <is>
-          <t>[20.7, 20.7, 20.7]</t>
+          <t>[20.7, 20.7]</t>
         </is>
       </c>
     </row>
@@ -21480,52 +21480,52 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10, 12]</t>
+          <t>[10, 10, 10, 12]</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>[28, 50, 30, 30, 32]</t>
+          <t>[28, 30, 30, 32]</t>
         </is>
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>[18, 40, 20, 20, 20]</t>
+          <t>[18, 20, 20, 20]</t>
         </is>
       </c>
       <c r="H293" t="inlineStr">
         <is>
-          <t>[162, 188, 147, 150, 51]</t>
+          <t>[162, 147, 150, 51]</t>
         </is>
       </c>
       <c r="I293" t="inlineStr">
         <is>
-          <t>[161.97, 188.47, 147.89, 150.24, 51.31]</t>
+          <t>[161.97, 147.89, 150.24, 51.31]</t>
         </is>
       </c>
       <c r="J293" t="inlineStr">
         <is>
-          <t>[135.48000000000002, 153.92999999999998, 126.08999999999999, 147.23000000000002, 51.31]</t>
+          <t>[135.48000000000002, 126.08999999999999, 147.23000000000002, 51.31]</t>
         </is>
       </c>
       <c r="K293" t="inlineStr">
         <is>
-          <t>[63.22, 91.29, 61.41, 61.16, 17.46]</t>
+          <t>[63.22, 61.41, 61.16, 17.46]</t>
         </is>
       </c>
       <c r="L293" t="inlineStr">
         <is>
-          <t>[116.59, 166.62, 143.96, 146.25, 102.07]</t>
+          <t>[116.59, 143.96, 146.25, 102.07]</t>
         </is>
       </c>
       <c r="M293" t="inlineStr">
         <is>
-          <t>[16776.86, 24841.1, 16797.33, 15751.69, 4465.25]</t>
+          <t>[16776.86, 16797.33, 15751.69, 4465.25]</t>
         </is>
       </c>
       <c r="N293" t="inlineStr">
         <is>
-          <t>[-15.83, -15.83, -15.83, -15.83, -15.83]</t>
+          <t>[-15.83, -15.83, -15.83, -15.83]</t>
         </is>
       </c>
     </row>
@@ -21624,52 +21624,52 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 10]</t>
+          <t>[10, 10, 10]</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>[30, 30, 32, 30]</t>
+          <t>[30, 32, 30]</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>[20, 20, 22, 20]</t>
+          <t>[20, 22, 20]</t>
         </is>
       </c>
       <c r="H295" t="inlineStr">
         <is>
-          <t>[115, 102, 82, 138]</t>
+          <t>[115, 82, 138]</t>
         </is>
       </c>
       <c r="I295" t="inlineStr">
         <is>
-          <t>[115.36, 102.62, 82.16, 138.84]</t>
+          <t>[115.36, 82.16, 138.84]</t>
         </is>
       </c>
       <c r="J295" t="inlineStr">
         <is>
-          <t>[99.94, 99.60000000000001, 78.81, 134.14000000000001]</t>
+          <t>[99.94, 78.81, 134.14000000000001]</t>
         </is>
       </c>
       <c r="K295" t="inlineStr">
         <is>
-          <t>[47.91, 42.91, 34.95, 56.48]</t>
+          <t>[47.91, 34.95, 56.48]</t>
         </is>
       </c>
       <c r="L295" t="inlineStr">
         <is>
-          <t>[147.63, 153.1, 131.43, 150.65]</t>
+          <t>[147.63, 131.43, 150.65]</t>
         </is>
       </c>
       <c r="M295" t="inlineStr">
         <is>
-          <t>[12849.97, 11426.93, 8332.99, 14825.37]</t>
+          <t>[12849.97, 8332.99, 14825.37]</t>
         </is>
       </c>
       <c r="N295" t="inlineStr">
         <is>
-          <t>[-1.61, -1.61, -1.61, -1.61]</t>
+          <t>[-1.61, -1.61, -1.61]</t>
         </is>
       </c>
     </row>
@@ -21912,52 +21912,52 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>[12, 10, 12]</t>
+          <t>[10, 12]</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>[30, 30, 34]</t>
+          <t>[30, 34]</t>
         </is>
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>[18, 20, 22]</t>
+          <t>[20, 22]</t>
         </is>
       </c>
       <c r="H299" t="inlineStr">
         <is>
-          <t>[113, 54, 48]</t>
+          <t>[54, 48]</t>
         </is>
       </c>
       <c r="I299" t="inlineStr">
         <is>
-          <t>[112.67999999999999, 53.989999999999995, 48.63]</t>
+          <t>[53.989999999999995, 48.63]</t>
         </is>
       </c>
       <c r="J299" t="inlineStr">
         <is>
-          <t>[99.27, 43.26, 45.61]</t>
+          <t>[43.26, 45.61]</t>
         </is>
       </c>
       <c r="K299" t="inlineStr">
         <is>
-          <t>[44.61, 18.61, 18.33]</t>
+          <t>[18.61, 18.33]</t>
         </is>
       </c>
       <c r="L299" t="inlineStr">
         <is>
-          <t>[138.92, 105.14, 131.18]</t>
+          <t>[105.14, 131.18]</t>
         </is>
       </c>
       <c r="M299" t="inlineStr">
         <is>
-          <t>[11906.65, 4909.01, 5009.73]</t>
+          <t>[4909.01, 5009.73]</t>
         </is>
       </c>
       <c r="N299" t="inlineStr">
         <is>
-          <t>[6.29, 6.29, 6.29]</t>
+          <t>[6.29, 6.29]</t>
         </is>
       </c>
     </row>
@@ -22416,52 +22416,52 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>[10, 12, 10, 12, 10]</t>
+          <t>[10, 10, 12, 10]</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>[30, 32, 30, 30, 30]</t>
+          <t>[30, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 18, 20]</t>
+          <t>[20, 20, 18, 20]</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
         <is>
-          <t>[85, 94, 97, 101, 99]</t>
+          <t>[85, 97, 101, 99]</t>
         </is>
       </c>
       <c r="I306" t="inlineStr">
         <is>
-          <t>[85.18, 94.24, 97.59, 101.61, 99.27]</t>
+          <t>[85.18, 97.59, 101.61, 99.27]</t>
         </is>
       </c>
       <c r="J306" t="inlineStr">
         <is>
-          <t>[79.14, 93.89999999999999, 94.57000000000001, 99.6, 86.85]</t>
+          <t>[79.14, 94.57000000000001, 99.6, 86.85]</t>
         </is>
       </c>
       <c r="K306" t="inlineStr">
         <is>
-          <t>[37.09, 39.56, 37.66, 44.25, 42.64]</t>
+          <t>[37.09, 37.66, 44.25, 42.64]</t>
         </is>
       </c>
       <c r="L306" t="inlineStr">
         <is>
-          <t>[197.67, 189.08, 125.89, 169.53, 156.49]</t>
+          <t>[197.67, 125.89, 169.53, 156.49]</t>
         </is>
       </c>
       <c r="M306" t="inlineStr">
         <is>
-          <t>[10907.08, 10793.96, 9268.85, 11735.87, 12124.47]</t>
+          <t>[10907.08, 9268.85, 11735.87, 12124.47]</t>
         </is>
       </c>
       <c r="N306" t="inlineStr">
         <is>
-          <t>[14.9, 14.9, 14.9, 14.9, 14.9]</t>
+          <t>[14.9, 14.9, 14.9, 14.9]</t>
         </is>
       </c>
     </row>
@@ -22488,52 +22488,52 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>[12, 12, 10, 12, 10]</t>
+          <t>[12, 10, 12, 10]</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>[30, 32, 30, 30, 30]</t>
+          <t>[32, 30, 30, 30]</t>
         </is>
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>[18, 20, 20, 18, 20]</t>
+          <t>[20, 20, 18, 20]</t>
         </is>
       </c>
       <c r="H307" t="inlineStr">
         <is>
-          <t>[79, 89, 117, 65, 97]</t>
+          <t>[89, 117, 65, 97]</t>
         </is>
       </c>
       <c r="I307" t="inlineStr">
         <is>
-          <t>[79.14, 89.2, 117.38, 65.06, 97.92]</t>
+          <t>[89.2, 117.38, 65.06, 97.92]</t>
         </is>
       </c>
       <c r="J307" t="inlineStr">
         <is>
-          <t>[74.44, 74.45, 99.6, 61.370000000000005, 84.84]</t>
+          <t>[74.45, 99.6, 61.370000000000005, 84.84]</t>
         </is>
       </c>
       <c r="K307" t="inlineStr">
         <is>
-          <t>[32.01, 36.29, 45.6, 25.3, 41.67]</t>
+          <t>[36.29, 45.6, 25.3, 41.67]</t>
         </is>
       </c>
       <c r="L307" t="inlineStr">
         <is>
-          <t>[151.35, 134.3, 114.16, 134.03, 151.75]</t>
+          <t>[134.3, 114.16, 134.03, 151.75]</t>
         </is>
       </c>
       <c r="M307" t="inlineStr">
         <is>
-          <t>[8399.24, 9393.37, 11614.77, 7184.29, 11171.72]</t>
+          <t>[9393.37, 11614.77, 7184.29, 11171.72]</t>
         </is>
       </c>
       <c r="N307" t="inlineStr">
         <is>
-          <t>[8.68, 8.68, 8.68, 8.68, 8.68]</t>
+          <t>[8.68, 8.68, 8.68, 8.68]</t>
         </is>
       </c>
     </row>
@@ -22632,52 +22632,52 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>[2, 12, 10, 12]</t>
+          <t>[12, 10, 12]</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>[28, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>[26, 18, 20, 18]</t>
+          <t>[18, 20, 18]</t>
         </is>
       </c>
       <c r="H309" t="inlineStr">
         <is>
-          <t>[134, 118, 195, 150]</t>
+          <t>[118, 195, 150]</t>
         </is>
       </c>
       <c r="I309" t="inlineStr">
         <is>
-          <t>[132.79999999999998, 117.71, 192.5, 149.9]</t>
+          <t>[117.71, 192.5, 149.9]</t>
         </is>
       </c>
       <c r="J309" t="inlineStr">
         <is>
-          <t>[127.1, 113.02, 191.49, 143.87]</t>
+          <t>[113.02, 191.49, 143.87]</t>
         </is>
       </c>
       <c r="K309" t="inlineStr">
         <is>
-          <t>[51.23, 46.56, 80.02, 53.3]</t>
+          <t>[46.56, 80.02, 53.3]</t>
         </is>
       </c>
       <c r="L309" t="inlineStr">
         <is>
-          <t>[99.78, 160.24, 91.58, 82.97]</t>
+          <t>[160.24, 91.58, 82.97]</t>
         </is>
       </c>
       <c r="M309" t="inlineStr">
         <is>
-          <t>[13174.48, 11611.99, 16960.43, 11905.26]</t>
+          <t>[11611.99, 16960.43, 11905.26]</t>
         </is>
       </c>
       <c r="N309" t="inlineStr">
         <is>
-          <t>[-9.89, -9.89, -9.89, -9.89]</t>
+          <t>[-9.89, -9.89, -9.89]</t>
         </is>
       </c>
     </row>
@@ -23064,52 +23064,52 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>[10, 10, 10, 16]</t>
+          <t>[10, 10, 16]</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>[30, 30, 30, 30]</t>
+          <t>[30, 30, 30]</t>
         </is>
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>[20, 20, 20, 14]</t>
+          <t>[20, 20, 14]</t>
         </is>
       </c>
       <c r="H315" t="inlineStr">
         <is>
-          <t>[214, 190, 205, 95]</t>
+          <t>[190, 205, 95]</t>
         </is>
       </c>
       <c r="I315" t="inlineStr">
         <is>
-          <t>[214.62, 189.81, 205.57, 94.89999999999999]</t>
+          <t>[189.81, 205.57, 94.89999999999999]</t>
         </is>
       </c>
       <c r="J315" t="inlineStr">
         <is>
-          <t>[194.17000000000002, 184.78, 204.23, 88.86999999999999]</t>
+          <t>[184.78, 204.23, 88.86999999999999]</t>
         </is>
       </c>
       <c r="K315" t="inlineStr">
         <is>
-          <t>[92.36, 73.58, 81.49, 35.53]</t>
+          <t>[73.58, 81.49, 35.53]</t>
         </is>
       </c>
       <c r="L315" t="inlineStr">
         <is>
-          <t>[142.26, 86.73, 97.72, 101.63]</t>
+          <t>[86.73, 97.72, 101.63]</t>
         </is>
       </c>
       <c r="M315" t="inlineStr">
         <is>
-          <t>[23078.23, 15373.98, 17544.58, 9357.91]</t>
+          <t>[15373.98, 17544.58, 9357.91]</t>
         </is>
       </c>
       <c r="N315" t="inlineStr">
         <is>
-          <t>[-6.55, -6.55, -6.55, -6.55]</t>
+          <t>[-6.55, -6.55, -6.55]</t>
         </is>
       </c>
     </row>
@@ -23352,52 +23352,52 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>[10, 10, 4]</t>
+          <t>[10, 4]</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t>[30, 30, 30]</t>
+          <t>[30, 30]</t>
         </is>
       </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>[20, 20, 26]</t>
+          <t>[20, 26]</t>
         </is>
       </c>
       <c r="H319" t="inlineStr">
         <is>
-          <t>[156, 218, 99]</t>
+          <t>[218, 99]</t>
         </is>
       </c>
       <c r="I319" t="inlineStr">
         <is>
-          <t>[155.94000000000003, 218.65, 98.6]</t>
+          <t>[218.65, 98.6]</t>
         </is>
       </c>
       <c r="J319" t="inlineStr">
         <is>
-          <t>[144.87, 212.28, 85.52]</t>
+          <t>[212.28, 85.52]</t>
         </is>
       </c>
       <c r="K319" t="inlineStr">
         <is>
-          <t>[62.88, 90.51, 30.81]</t>
+          <t>[90.51, 30.81]</t>
         </is>
       </c>
       <c r="L319" t="inlineStr">
         <is>
-          <t>[125.56, 102.67, 60.2]</t>
+          <t>[102.67, 60.2]</t>
         </is>
       </c>
       <c r="M319" t="inlineStr">
         <is>
-          <t>[14797.08, 20013.01, 6821.06]</t>
+          <t>[20013.01, 6821.06]</t>
         </is>
       </c>
       <c r="N319" t="inlineStr">
         <is>
-          <t>[11.84, 11.84, 11.84]</t>
+          <t>[11.84, 11.84]</t>
         </is>
       </c>
     </row>
@@ -23568,52 +23568,52 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>[10, 10, 14, 14]</t>
+          <t>[10, 14, 14]</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>[30, 30, 28, 32]</t>
+          <t>[30, 28, 32]</t>
         </is>
       </c>
       <c r="G322" t="inlineStr">
         <is>
-          <t>[20, 20, 14, 18]</t>
+          <t>[20, 14, 18]</t>
         </is>
       </c>
       <c r="H322" t="inlineStr">
         <is>
-          <t>[223, 212, 50, 59]</t>
+          <t>[212, 50, 59]</t>
         </is>
       </c>
       <c r="I322" t="inlineStr">
         <is>
-          <t>[223.01, 212.28, 49.96, 59.36]</t>
+          <t>[212.28, 49.96, 59.36]</t>
         </is>
       </c>
       <c r="J322" t="inlineStr">
         <is>
-          <t>[183.44, 183.44, 39.9, 51.31]</t>
+          <t>[183.44, 39.9, 51.31]</t>
         </is>
       </c>
       <c r="K322" t="inlineStr">
         <is>
-          <t>[89.86, 79.69, 17.14, 19.18]</t>
+          <t>[79.69, 17.14, 19.18]</t>
         </is>
       </c>
       <c r="L322" t="inlineStr">
         <is>
-          <t>[149.5, 93.77, 72.86, 75.3]</t>
+          <t>[93.77, 72.86, 75.3]</t>
         </is>
       </c>
       <c r="M322" t="inlineStr">
         <is>
-          <t>[24056.81, 16982.62, 5112.47, 4370.55]</t>
+          <t>[16982.62, 5112.47, 4370.55]</t>
         </is>
       </c>
       <c r="N322" t="inlineStr">
         <is>
-          <t>[9.33, 9.33, 9.33, 9.33]</t>
+          <t>[9.33, 9.33, 9.33]</t>
         </is>
       </c>
     </row>

</xml_diff>